<commit_message>
added multiple functions, working on scraping dropdowns
</commit_message>
<xml_diff>
--- a/PANDAS PROJ/RECDCF.xlsx
+++ b/PANDAS PROJ/RECDCF.xlsx
@@ -8,16 +8,48 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Downloads\SPRING SEMESTER 2021-2022\PYTHON\GitHub\steveproject\PANDAS PROJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FD613A-0A7D-472E-8FD2-25198B9C7D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EAD81E-2A87-4377-BC55-0E7A85402AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{38F17426-425A-4946-BB5F-3622334B00E1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{38F17426-425A-4946-BB5F-3622334B00E1}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="6" r:id="rId1"/>
     <sheet name="DCF" sheetId="1" r:id="rId2"/>
     <sheet name="WACC" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <definedNames>
+    <definedName name="IQ_CH">110000</definedName>
+    <definedName name="IQ_CQ">5000</definedName>
+    <definedName name="IQ_CY">10000</definedName>
+    <definedName name="IQ_DAILY">500000</definedName>
+    <definedName name="IQ_DNTM" hidden="1">700000</definedName>
+    <definedName name="IQ_FH">100000</definedName>
+    <definedName name="IQ_FQ">500</definedName>
+    <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
+    <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
+    <definedName name="IQ_FWD_CY2" hidden="1">10003</definedName>
+    <definedName name="IQ_FWD_FY" hidden="1">1001</definedName>
+    <definedName name="IQ_FWD_FY1" hidden="1">1002</definedName>
+    <definedName name="IQ_FWD_FY2" hidden="1">1003</definedName>
+    <definedName name="IQ_FWD_Q" hidden="1">501</definedName>
+    <definedName name="IQ_FWD_Q1" hidden="1">502</definedName>
+    <definedName name="IQ_FWD_Q2" hidden="1">503</definedName>
+    <definedName name="IQ_FY">1000</definedName>
+    <definedName name="IQ_LATESTK" hidden="1">1000</definedName>
+    <definedName name="IQ_LATESTQ" hidden="1">500</definedName>
+    <definedName name="IQ_LTM">2000</definedName>
+    <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
+    <definedName name="IQ_MONTH">15000</definedName>
+    <definedName name="IQ_MTD" hidden="1">800000</definedName>
+    <definedName name="IQ_NAMES_REVISION_DATE_" hidden="1">44651.1399421296</definedName>
+    <definedName name="IQ_NTM">6000</definedName>
+    <definedName name="IQ_QTD" hidden="1">750000</definedName>
+    <definedName name="IQ_TODAY" hidden="1">0</definedName>
+    <definedName name="IQ_WEEK">50000</definedName>
+    <definedName name="IQ_YTD">3000</definedName>
+    <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
+  </definedNames>
+  <calcPr calcId="191028" calcMode="manual" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
   <si>
     <t>Discounted Cash Flow Valuation</t>
   </si>
@@ -158,12 +190,6 @@
     <t>Short Term liabilities</t>
   </si>
   <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>Cash Equivalents</t>
-  </si>
-  <si>
     <t>Net Debt</t>
   </si>
   <si>
@@ -266,12 +292,6 @@
     <t>NWC</t>
   </si>
   <si>
-    <t xml:space="preserve">cost of debt </t>
-  </si>
-  <si>
-    <t>(just the most recent)</t>
-  </si>
-  <si>
     <t>Todays date</t>
   </si>
   <si>
@@ -281,9 +301,6 @@
     <t>Current Price</t>
   </si>
   <si>
-    <t xml:space="preserve">RF rate </t>
-  </si>
-  <si>
     <t>RF Rate</t>
   </si>
   <si>
@@ -302,12 +319,6 @@
     <t>Exit Mult</t>
   </si>
   <si>
-    <t xml:space="preserve">grab the name of the company </t>
-  </si>
-  <si>
-    <t xml:space="preserve">grab the units of all financial statements? </t>
-  </si>
-  <si>
     <t>&lt; these default to moving averages please account for your subjective assumptions</t>
   </si>
   <si>
@@ -326,10 +337,10 @@
     <t xml:space="preserve">Cash + Cash Equivalents </t>
   </si>
   <si>
-    <t>CSX</t>
-  </si>
-  <si>
-    <t>CSX Corporation (CSX)</t>
+    <t>CSL</t>
+  </si>
+  <si>
+    <t>Carlisle Companies Incorporated (CSL)</t>
   </si>
 </sst>
 </file>
@@ -777,7 +788,7 @@
     <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -948,12 +959,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="20" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="10" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -991,9 +999,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>479307</xdr:colOff>
+      <xdr:colOff>475497</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>158107</xdr:rowOff>
+      <xdr:rowOff>169537</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1328,17 +1336,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CEE626-EE9B-4164-BEB3-9EE6EF61F1A8}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="36.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1355,7 +1362,7 @@
       </c>
       <c r="E1" s="92"/>
       <c r="F1" s="93" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1363,19 +1370,19 @@
         <v>12</v>
       </c>
       <c r="B2" s="95">
-        <v>12522000</v>
+        <v>4810000</v>
       </c>
       <c r="C2" s="95">
-        <v>10583000</v>
+        <v>3970000</v>
       </c>
       <c r="D2" s="95">
-        <v>11937000</v>
+        <v>4810000</v>
       </c>
       <c r="E2" s="86" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F2" s="96" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G2" s="78"/>
     </row>
@@ -1384,19 +1391,19 @@
         <v>14</v>
       </c>
       <c r="B3" s="86">
-        <v>7093000</v>
+        <v>837800</v>
       </c>
       <c r="C3" s="86">
-        <v>5764000</v>
+        <v>762200</v>
       </c>
       <c r="D3" s="86">
-        <v>6402000</v>
+        <v>861900</v>
       </c>
       <c r="E3" s="86" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F3" s="96">
-        <v>44641</v>
+        <v>44659</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16.2" thickBot="1">
@@ -1404,22 +1411,22 @@
         <v>16</v>
       </c>
       <c r="B4" s="95">
-        <v>5673000</v>
+        <v>584500</v>
       </c>
       <c r="C4" s="95">
-        <v>4381000</v>
+        <v>509900</v>
       </c>
       <c r="D4" s="95">
-        <v>5053000</v>
+        <v>656500</v>
       </c>
       <c r="E4" s="86" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F4" s="97">
-        <v>36.86</v>
+        <v>235</v>
       </c>
       <c r="H4" s="101" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I4" s="102"/>
       <c r="J4" s="102"/>
@@ -1428,185 +1435,185 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="94" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="95">
-        <v>1170000</v>
+        <v>482500</v>
       </c>
       <c r="C5" s="95">
-        <v>862000</v>
+        <v>404200</v>
       </c>
       <c r="D5" s="95">
-        <v>985000</v>
+        <v>595300</v>
       </c>
       <c r="E5" s="86" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="97">
-        <v>1.22</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="94" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="95">
-        <v>3781000</v>
+        <v>95500</v>
       </c>
       <c r="C6" s="95">
-        <v>2765000</v>
+        <v>78500</v>
       </c>
       <c r="D6" s="95">
-        <v>3331000</v>
+        <v>121600</v>
       </c>
       <c r="E6" s="86" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F6" s="97">
-        <v>2.315E-2</v>
+        <v>2.6520000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="94" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="95">
-        <v>-1791000</v>
+        <v>-134800</v>
       </c>
       <c r="C7" s="95">
-        <v>-1626000</v>
+        <v>-95500</v>
       </c>
       <c r="D7" s="95">
-        <v>-1657000</v>
+        <v>-88900</v>
       </c>
       <c r="E7" s="86" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" s="97">
-        <v>0</v>
+        <v>3.0416666666666668E-2</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="94" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="95">
-        <v>1640000</v>
+        <v>980000</v>
       </c>
       <c r="C8" s="95">
-        <v>2422000</v>
+        <v>1563800</v>
       </c>
       <c r="D8" s="95">
-        <v>1127000</v>
+        <v>851000</v>
       </c>
       <c r="E8" s="86" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F8" s="97">
-        <v>0</v>
-      </c>
-      <c r="G8" s="110"/>
+        <v>3450000</v>
+      </c>
+      <c r="G8" s="109"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="94" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B9" s="86"/>
       <c r="C9" s="86"/>
       <c r="D9" s="86"/>
       <c r="E9" s="86" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F9" s="97">
-        <v>1</v>
-      </c>
-      <c r="G9" s="110"/>
+        <v>1170000</v>
+      </c>
+      <c r="G9" s="109"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="94" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B10" s="86"/>
       <c r="C10" s="86"/>
       <c r="D10" s="86"/>
       <c r="E10" s="86" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F10" s="97">
-        <v>2</v>
-      </c>
-      <c r="G10" s="110"/>
+        <v>324400</v>
+      </c>
+      <c r="G10" s="109"/>
       <c r="H10" s="86"/>
       <c r="I10" s="86"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="94" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B11" s="86"/>
       <c r="C11" s="86"/>
       <c r="D11" s="86"/>
       <c r="E11" s="86" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="97">
-        <v>4</v>
+        <v>80</v>
+      </c>
+      <c r="F11" s="110">
+        <v>52068.085106382976</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="94" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B12" s="86"/>
       <c r="C12" s="86"/>
       <c r="D12" s="86"/>
       <c r="E12" s="86" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F12" s="97">
-        <v>5</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="94" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B13" s="86"/>
       <c r="C13" s="86"/>
       <c r="D13" s="86"/>
       <c r="E13" s="86" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F13" s="97">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="94" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B14" s="86"/>
       <c r="C14" s="86"/>
       <c r="D14" s="86"/>
       <c r="E14" s="86" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F14" s="97" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="16.2" thickBot="1">
       <c r="A15" s="98" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B15" s="99"/>
       <c r="C15" s="99"/>
       <c r="D15" s="99"/>
       <c r="E15" s="99" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F15" s="100" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1619,62 +1626,48 @@
       <c r="A18" s="1"/>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="105" t="s">
-        <v>88</v>
-      </c>
+      <c r="A19" s="105"/>
+      <c r="B19" s="86"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>89</v>
-      </c>
+      <c r="A20" s="86"/>
+      <c r="B20" s="86"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>81</v>
-      </c>
+      <c r="A21" s="86"/>
+      <c r="B21" s="86"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="94" t="s">
-        <v>76</v>
-      </c>
+      <c r="A22" s="86"/>
+      <c r="B22" s="86"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="86"/>
+      <c r="B23" s="86"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>77</v>
-      </c>
+      <c r="A24" s="25"/>
+      <c r="B24" s="86"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>77</v>
-      </c>
+      <c r="A25" s="25"/>
+      <c r="B25" s="86"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>77</v>
-      </c>
+      <c r="A26" s="25"/>
+      <c r="B26" s="86"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" t="s">
-        <v>77</v>
-      </c>
+      <c r="A27" s="25"/>
+      <c r="B27" s="86"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="94"/>
-    </row>
-    <row r="29" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A29" s="98"/>
+      <c r="A28" s="86"/>
+      <c r="B28" s="86"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="86"/>
+      <c r="B29" s="86"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1684,10 +1677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF651AB-D597-9D44-826B-59063E0D92DF}">
-  <dimension ref="B2:N85"/>
+  <dimension ref="B2:N86"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4"/>
@@ -1738,7 +1731,7 @@
       </c>
       <c r="G5" s="36">
         <f>WACC!F18</f>
-        <v>0.13135797358695675</v>
+        <v>9.3840028571543804E-2</v>
       </c>
       <c r="H5" s="19"/>
     </row>
@@ -1748,14 +1741,14 @@
       </c>
       <c r="C6" s="104" t="str">
         <f>DATA!F2</f>
-        <v>CSX</v>
+        <v>CSL</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="8">
         <f>DATA!F4</f>
-        <v>36.86</v>
+        <v>235</v>
       </c>
       <c r="I6" s="7"/>
     </row>
@@ -1772,7 +1765,7 @@
       </c>
       <c r="G7" s="5">
         <f>DATA!F3</f>
-        <v>44641</v>
+        <v>44659</v>
       </c>
     </row>
     <row r="8" spans="2:12">
@@ -1789,7 +1782,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5">
         <f>G7</f>
-        <v>44641</v>
+        <v>44659</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -1896,40 +1889,37 @@
       </c>
       <c r="C15" s="9">
         <f>DATA!D2</f>
-        <v>11937000</v>
+        <v>4810000</v>
       </c>
       <c r="D15" s="9">
         <f>DATA!C2</f>
-        <v>10583000</v>
+        <v>3970000</v>
       </c>
       <c r="E15" s="9">
         <f>DATA!B2</f>
-        <v>12522000</v>
+        <v>4810000</v>
       </c>
       <c r="F15" s="10">
         <f>E15*(1+F16)</f>
-        <v>13774200.000000002</v>
+        <v>4898866.4987405548</v>
       </c>
       <c r="G15" s="10">
-        <f t="shared" ref="G15:K15" si="2">F15*(1+G16)</f>
-        <v>15151620.000000004</v>
+        <f t="shared" ref="G15:J15" si="2">F15*(1+G16)</f>
+        <v>4989374.8383539589</v>
       </c>
       <c r="H15" s="10">
         <f t="shared" si="2"/>
-        <v>16666782.000000006</v>
+        <v>5402723.9690103875</v>
       </c>
       <c r="I15" s="10">
         <f t="shared" si="2"/>
-        <v>18333460.200000007</v>
+        <v>5618466.6292516654</v>
       </c>
       <c r="J15" s="10">
         <f t="shared" si="2"/>
-        <v>20166806.22000001</v>
-      </c>
-      <c r="K15" s="10">
-        <f t="shared" si="2"/>
-        <v>20166806.22000001</v>
-      </c>
+        <v>5883009.2107630614</v>
+      </c>
+      <c r="K15" s="10"/>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="3" t="s">
@@ -1938,26 +1928,31 @@
       <c r="C16" s="12"/>
       <c r="D16" s="12">
         <f>(D15-C15)/C15</f>
-        <v>-0.11342883471559018</v>
+        <v>-0.17463617463617465</v>
       </c>
       <c r="E16" s="12">
         <f>(E15-D15)/D15</f>
-        <v>0.18321836908249078</v>
-      </c>
-      <c r="F16" s="108">
-        <v>0.1</v>
-      </c>
-      <c r="G16" s="108">
-        <v>0.1</v>
-      </c>
-      <c r="H16" s="108">
-        <v>0.1</v>
-      </c>
-      <c r="I16" s="108">
-        <v>0.1</v>
-      </c>
-      <c r="J16" s="108">
-        <v>0.1</v>
+        <v>0.21158690176322417</v>
+      </c>
+      <c r="F16" s="107">
+        <f>AVERAGE(C16:E16)</f>
+        <v>1.8475363563524763E-2</v>
+      </c>
+      <c r="G16" s="107">
+        <f t="shared" ref="G16" si="3">AVERAGE(D16:F16)</f>
+        <v>1.8475363563524763E-2</v>
+      </c>
+      <c r="H16" s="107">
+        <f t="shared" ref="H16" si="4">AVERAGE(E16:G16)</f>
+        <v>8.2845876296757895E-2</v>
+      </c>
+      <c r="I16" s="107">
+        <f t="shared" ref="I16" si="5">AVERAGE(F16:H16)</f>
+        <v>3.9932201141269143E-2</v>
+      </c>
+      <c r="J16" s="107">
+        <f t="shared" ref="J16" si="6">AVERAGE(G16:I16)</f>
+        <v>4.7084480333850598E-2</v>
       </c>
     </row>
     <row r="17" spans="2:12">
@@ -1966,35 +1961,35 @@
       </c>
       <c r="C17" s="9">
         <f>DATA!D3</f>
-        <v>6402000</v>
+        <v>861900</v>
       </c>
       <c r="D17" s="9">
         <f>DATA!C3</f>
-        <v>5764000</v>
+        <v>762200</v>
       </c>
       <c r="E17" s="9">
         <f>DATA!B3</f>
-        <v>7093000</v>
+        <v>837800</v>
       </c>
       <c r="F17" s="10">
         <f>F15*F18</f>
-        <v>7300326.0000000009</v>
+        <v>890545.1947835664</v>
       </c>
       <c r="G17" s="10">
-        <f t="shared" ref="G17:J17" si="3">G15*G18</f>
-        <v>8030358.6000000024</v>
+        <f t="shared" ref="G17:J17" si="7">G15*G18</f>
+        <v>911317.11075406126</v>
       </c>
       <c r="H17" s="10">
-        <f t="shared" si="3"/>
-        <v>8833394.4600000028</v>
+        <f t="shared" si="7"/>
+        <v>969998.44499027822</v>
       </c>
       <c r="I17" s="10">
-        <f t="shared" si="3"/>
-        <v>9716733.9060000032</v>
+        <f t="shared" si="7"/>
+        <v>1018770.9097975146</v>
       </c>
       <c r="J17" s="10">
-        <f t="shared" si="3"/>
-        <v>10688407.296600007</v>
+        <f t="shared" si="7"/>
+        <v>1065836.1010241969</v>
       </c>
     </row>
     <row r="18" spans="2:12">
@@ -2003,33 +1998,38 @@
       </c>
       <c r="C18" s="13">
         <f>C17/C15</f>
-        <v>0.53631565720030161</v>
+        <v>0.17918918918918919</v>
       </c>
       <c r="D18" s="13">
-        <f t="shared" ref="D18:J18" si="4">D17/D15</f>
-        <v>0.54464707549844094</v>
+        <f t="shared" ref="D18:E18" si="8">D17/D15</f>
+        <v>0.19198992443324936</v>
       </c>
       <c r="E18" s="13">
-        <f t="shared" si="4"/>
-        <v>0.56644306021402335</v>
+        <f t="shared" si="8"/>
+        <v>0.17417879417879417</v>
       </c>
       <c r="F18" s="107">
-        <v>0.53</v>
+        <f>AVERAGE(C18:E18)</f>
+        <v>0.18178596926707757</v>
       </c>
       <c r="G18" s="107">
-        <v>0.53</v>
+        <f t="shared" ref="G18:J18" si="9">AVERAGE(D18:F18)</f>
+        <v>0.18265156262637369</v>
       </c>
       <c r="H18" s="107">
-        <v>0.53</v>
+        <f t="shared" si="9"/>
+        <v>0.17953877535741514</v>
       </c>
       <c r="I18" s="107">
-        <v>0.53</v>
+        <f t="shared" si="9"/>
+        <v>0.18132543575028881</v>
       </c>
       <c r="J18" s="107">
-        <v>0.53</v>
-      </c>
-      <c r="L18" s="109" t="s">
-        <v>90</v>
+        <f t="shared" si="9"/>
+        <v>0.18117192457802589</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="2:12">
@@ -2038,35 +2038,35 @@
       </c>
       <c r="C19" s="9">
         <f>DATA!D4</f>
-        <v>5053000</v>
+        <v>656500</v>
       </c>
       <c r="D19" s="9">
         <f>DATA!C4</f>
-        <v>4381000</v>
+        <v>509900</v>
       </c>
       <c r="E19" s="9">
         <f>DATA!B4</f>
-        <v>5673000</v>
+        <v>584500</v>
       </c>
       <c r="F19" s="10">
         <f>F15*F20</f>
-        <v>5785164.0000000009</v>
+        <v>631043.31609166053</v>
       </c>
       <c r="G19" s="10">
-        <f t="shared" ref="G19:J19" si="5">G15*G20</f>
-        <v>6363680.4000000013</v>
+        <f t="shared" ref="G19:J19" si="10">G15*G20</f>
+        <v>629942.01389071054</v>
       </c>
       <c r="H19" s="10">
-        <f t="shared" si="5"/>
-        <v>7000048.4400000023</v>
+        <f t="shared" si="10"/>
+        <v>678201.27854894917</v>
       </c>
       <c r="I19" s="10">
-        <f t="shared" si="5"/>
-        <v>7700053.2840000028</v>
+        <f t="shared" si="10"/>
+        <v>712796.80379550753</v>
       </c>
       <c r="J19" s="10">
-        <f t="shared" si="5"/>
-        <v>8470058.6124000046</v>
+        <f t="shared" si="10"/>
+        <v>742539.68737077643</v>
       </c>
     </row>
     <row r="20" spans="2:12">
@@ -2075,104 +2075,109 @@
       </c>
       <c r="C20" s="13">
         <f>C19/C15</f>
-        <v>0.42330568819636427</v>
+        <v>0.13648648648648648</v>
       </c>
       <c r="D20" s="13">
         <f>D19/D15</f>
-        <v>0.41396579419824248</v>
+        <v>0.12843828715365238</v>
       </c>
       <c r="E20" s="13">
         <f>E19/E15</f>
-        <v>0.45304264494489699</v>
+        <v>0.12151767151767152</v>
       </c>
       <c r="F20" s="107">
-        <v>0.42</v>
+        <f>AVERAGE(C20:E20)</f>
+        <v>0.1288141483859368</v>
       </c>
       <c r="G20" s="107">
-        <v>0.42</v>
+        <f t="shared" ref="G20" si="11">AVERAGE(D20:F20)</f>
+        <v>0.12625670235242023</v>
       </c>
       <c r="H20" s="107">
-        <v>0.42</v>
+        <f t="shared" ref="H20" si="12">AVERAGE(E20:G20)</f>
+        <v>0.12552950741867619</v>
       </c>
       <c r="I20" s="107">
-        <v>0.42</v>
+        <f t="shared" ref="I20" si="13">AVERAGE(F20:H20)</f>
+        <v>0.12686678605234439</v>
       </c>
       <c r="J20" s="107">
-        <v>0.42</v>
+        <f t="shared" ref="J20" si="14">AVERAGE(G20:I20)</f>
+        <v>0.12621766527448028</v>
       </c>
     </row>
     <row r="22" spans="2:12">
       <c r="B22" s="79" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="9">
         <f>DATA!D5</f>
-        <v>985000</v>
+        <v>595300</v>
       </c>
       <c r="D22" s="9">
         <f>DATA!C5</f>
-        <v>862000</v>
+        <v>404200</v>
       </c>
       <c r="E22" s="9">
         <f>DATA!B5</f>
-        <v>1170000</v>
+        <v>482500</v>
       </c>
       <c r="F22" s="87">
         <f>F19</f>
-        <v>5785164.0000000009</v>
+        <v>631043.31609166053</v>
       </c>
       <c r="G22" s="87">
-        <f t="shared" ref="G22:J22" si="6">G19</f>
-        <v>6363680.4000000013</v>
+        <f t="shared" ref="G22:J22" si="15">G19</f>
+        <v>629942.01389071054</v>
       </c>
       <c r="H22" s="87">
-        <f t="shared" si="6"/>
-        <v>7000048.4400000023</v>
+        <f t="shared" si="15"/>
+        <v>678201.27854894917</v>
       </c>
       <c r="I22" s="87">
-        <f t="shared" si="6"/>
-        <v>7700053.2840000028</v>
+        <f t="shared" si="15"/>
+        <v>712796.80379550753</v>
       </c>
       <c r="J22" s="87">
-        <f t="shared" si="6"/>
-        <v>8470058.6124000046</v>
+        <f t="shared" si="15"/>
+        <v>742539.68737077643</v>
       </c>
     </row>
     <row r="23" spans="2:12">
       <c r="B23" s="79" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" s="9">
         <f>DATA!D6</f>
-        <v>3331000</v>
+        <v>121600</v>
       </c>
       <c r="D23" s="9">
         <f>DATA!C6</f>
-        <v>2765000</v>
+        <v>78500</v>
       </c>
       <c r="E23" s="9">
         <f>DATA!B6</f>
-        <v>3781000</v>
+        <v>95500</v>
       </c>
       <c r="F23" s="87">
         <f>F22*F24</f>
-        <v>-115703.28000000003</v>
+        <v>125452.46384798236</v>
       </c>
       <c r="G23" s="87">
-        <f t="shared" ref="G23:J23" si="7">G22*G24</f>
-        <v>-127273.60800000002</v>
+        <f t="shared" ref="G23:J23" si="16">G22*G24</f>
+        <v>124085.96024198929</v>
       </c>
       <c r="H23" s="87">
-        <f t="shared" si="7"/>
-        <v>-140000.96880000006</v>
+        <f t="shared" si="16"/>
+        <v>134218.09049768021</v>
       </c>
       <c r="I23" s="87">
-        <f t="shared" si="7"/>
-        <v>-154001.06568000006</v>
+        <f t="shared" si="16"/>
+        <v>141058.84596819282</v>
       </c>
       <c r="J23" s="87">
-        <f t="shared" si="7"/>
-        <v>-169401.1722480001</v>
+        <f t="shared" si="16"/>
+        <v>146720.37142515319</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -2181,30 +2186,35 @@
       </c>
       <c r="C24" s="88">
         <f>C23/C22</f>
-        <v>3.3817258883248731</v>
+        <v>0.20426675625734925</v>
       </c>
       <c r="D24" s="88">
-        <f t="shared" ref="D24:E24" si="8">D23/D22</f>
-        <v>3.2076566125290022</v>
+        <f t="shared" ref="D24:E24" si="17">D23/D22</f>
+        <v>0.194210786739238</v>
       </c>
       <c r="E24" s="88">
-        <f t="shared" si="8"/>
-        <v>3.2316239316239317</v>
-      </c>
-      <c r="F24" s="111">
-        <v>-0.02</v>
-      </c>
-      <c r="G24" s="111">
-        <v>-0.02</v>
-      </c>
-      <c r="H24" s="111">
-        <v>-0.02</v>
-      </c>
-      <c r="I24" s="111">
-        <v>-0.02</v>
-      </c>
-      <c r="J24" s="111">
-        <v>-0.02</v>
+        <f t="shared" si="17"/>
+        <v>0.19792746113989637</v>
+      </c>
+      <c r="F24" s="107">
+        <f>AVERAGE(C24:E24)</f>
+        <v>0.19880166804549451</v>
+      </c>
+      <c r="G24" s="107">
+        <f t="shared" ref="G24" si="18">AVERAGE(D24:F24)</f>
+        <v>0.19697997197487629</v>
+      </c>
+      <c r="H24" s="107">
+        <f t="shared" ref="H24" si="19">AVERAGE(E24:G24)</f>
+        <v>0.19790303372008908</v>
+      </c>
+      <c r="I24" s="107">
+        <f t="shared" ref="I24" si="20">AVERAGE(F24:H24)</f>
+        <v>0.19789489124681994</v>
+      </c>
+      <c r="J24" s="107">
+        <f t="shared" ref="J24" si="21">AVERAGE(G24:I24)</f>
+        <v>0.19759263231392843</v>
       </c>
     </row>
     <row r="25" spans="2:12">
@@ -2213,35 +2223,35 @@
       </c>
       <c r="C25" s="81">
         <f>C19*(1-C24)</f>
-        <v>-12034860.913705584</v>
+        <v>522398.87451705022</v>
       </c>
       <c r="D25" s="81">
-        <f t="shared" ref="D25:J25" si="9">D19*(1-D24)</f>
-        <v>-9671743.619489558</v>
+        <f t="shared" ref="D25:J25" si="22">D19*(1-D24)</f>
+        <v>410871.91984166257</v>
       </c>
       <c r="E25" s="81">
-        <f t="shared" si="9"/>
-        <v>-12660002.564102564</v>
+        <f t="shared" si="22"/>
+        <v>468811.39896373061</v>
       </c>
       <c r="F25" s="81">
-        <f t="shared" si="9"/>
-        <v>5900867.2800000012</v>
+        <f t="shared" si="22"/>
+        <v>505590.85224367818</v>
       </c>
       <c r="G25" s="81">
-        <f t="shared" si="9"/>
-        <v>6490954.0080000013</v>
+        <f t="shared" si="22"/>
+        <v>505856.05364872125</v>
       </c>
       <c r="H25" s="81">
-        <f t="shared" si="9"/>
-        <v>7140049.4088000022</v>
+        <f t="shared" si="22"/>
+        <v>543983.18805126892</v>
       </c>
       <c r="I25" s="81">
-        <f t="shared" si="9"/>
-        <v>7854054.3496800028</v>
+        <f t="shared" si="22"/>
+        <v>571737.95782731473</v>
       </c>
       <c r="J25" s="81">
-        <f t="shared" si="9"/>
-        <v>8639459.7846480049</v>
+        <f t="shared" si="22"/>
+        <v>595819.31594562321</v>
       </c>
     </row>
     <row r="27" spans="2:12">
@@ -2250,35 +2260,35 @@
       </c>
       <c r="C27" s="10">
         <f>C17-C19</f>
-        <v>1349000</v>
+        <v>205400</v>
       </c>
       <c r="D27" s="10">
         <f>D17-D19</f>
-        <v>1383000</v>
+        <v>252300</v>
       </c>
       <c r="E27" s="10">
-        <f t="shared" ref="E27:J27" si="10">E17-E19</f>
-        <v>1420000</v>
+        <f t="shared" ref="E27:J27" si="23">E17-E19</f>
+        <v>253300</v>
       </c>
       <c r="F27" s="10">
-        <f t="shared" si="10"/>
-        <v>1515162</v>
+        <f t="shared" si="23"/>
+        <v>259501.87869190588</v>
       </c>
       <c r="G27" s="10">
-        <f t="shared" si="10"/>
-        <v>1666678.2000000011</v>
+        <f t="shared" si="23"/>
+        <v>281375.09686335071</v>
       </c>
       <c r="H27" s="10">
-        <f t="shared" si="10"/>
-        <v>1833346.0200000005</v>
+        <f t="shared" si="23"/>
+        <v>291797.16644132906</v>
       </c>
       <c r="I27" s="10">
-        <f t="shared" si="10"/>
-        <v>2016680.6220000004</v>
+        <f t="shared" si="23"/>
+        <v>305974.10600200703</v>
       </c>
       <c r="J27" s="10">
-        <f t="shared" si="10"/>
-        <v>2218348.6842000019</v>
+        <f t="shared" si="23"/>
+        <v>323296.41365342052</v>
       </c>
     </row>
     <row r="28" spans="2:12">
@@ -2287,32 +2297,32 @@
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10">
-        <f t="shared" ref="D28:J28" si="11">C34-D34</f>
-        <v>-1295000</v>
+        <f t="shared" ref="D28:J28" si="24">C34-D34</f>
+        <v>-712800</v>
       </c>
       <c r="E28" s="10">
         <f>D34-E34</f>
-        <v>782000</v>
+        <v>583800</v>
       </c>
       <c r="F28" s="10">
-        <f t="shared" si="11"/>
-        <v>-1114840.0000000005</v>
+        <f t="shared" si="24"/>
+        <v>-284837.62735089799</v>
       </c>
       <c r="G28" s="10">
-        <f t="shared" si="11"/>
-        <v>-275484.00000000047</v>
+        <f t="shared" si="24"/>
+        <v>-158525.13969442388</v>
       </c>
       <c r="H28" s="10">
-        <f t="shared" si="11"/>
-        <v>-303032.40000000037</v>
+        <f t="shared" si="24"/>
+        <v>77704.798847240862</v>
       </c>
       <c r="I28" s="10">
-        <f t="shared" si="11"/>
-        <v>-333335.64000000013</v>
+        <f t="shared" si="24"/>
+        <v>-138626.5113720214</v>
       </c>
       <c r="J28" s="10">
-        <f t="shared" si="11"/>
-        <v>-366669.20400000084</v>
+        <f t="shared" si="24"/>
+        <v>-81632.747461109422</v>
       </c>
     </row>
     <row r="29" spans="2:12">
@@ -2321,35 +2331,35 @@
       </c>
       <c r="C29" s="9">
         <f>DATA!D7*-1</f>
-        <v>1657000</v>
+        <v>88900</v>
       </c>
       <c r="D29" s="9">
         <f>DATA!C7*-1</f>
-        <v>1626000</v>
+        <v>95500</v>
       </c>
       <c r="E29" s="9">
         <f>DATA!B7*-1</f>
-        <v>1791000</v>
+        <v>134800</v>
       </c>
       <c r="F29" s="10">
         <f>-(F15*F30)</f>
-        <v>1377420.0000000002</v>
+        <v>59614.757947251652</v>
       </c>
       <c r="G29" s="10">
-        <f t="shared" ref="G29:J29" si="12">-(G15*G30)</f>
-        <v>1515162.0000000005</v>
+        <f t="shared" ref="G29:J29" si="25">-(G15*G30)</f>
+        <v>50216.461470797411</v>
       </c>
       <c r="H29" s="10">
-        <f t="shared" si="12"/>
-        <v>1666678.2000000007</v>
+        <f t="shared" si="25"/>
+        <v>90511.330864525298</v>
       </c>
       <c r="I29" s="10">
-        <f t="shared" si="12"/>
-        <v>1833346.0200000007</v>
+        <f t="shared" si="25"/>
+        <v>73015.118290667669</v>
       </c>
       <c r="J29" s="10">
-        <f t="shared" si="12"/>
-        <v>2016680.6220000011</v>
+        <f t="shared" si="25"/>
+        <v>78073.702483399888</v>
       </c>
     </row>
     <row r="30" spans="2:12">
@@ -2358,29 +2368,34 @@
       </c>
       <c r="C30" s="13">
         <f>-(C29/C15)</f>
-        <v>-0.13881209684175252</v>
+        <v>-1.8482328482328482E-2</v>
       </c>
       <c r="D30" s="13">
         <v>0.01</v>
       </c>
       <c r="E30" s="13">
-        <f t="shared" ref="E30" si="13">-(E29/E15)</f>
-        <v>-0.1430282702443699</v>
+        <f t="shared" ref="E30" si="26">-(E29/E15)</f>
+        <v>-2.8024948024948024E-2</v>
       </c>
       <c r="F30" s="107">
-        <v>-0.1</v>
+        <f>AVERAGE(C30:E30)</f>
+        <v>-1.2169092169092168E-2</v>
       </c>
       <c r="G30" s="107">
-        <v>-0.1</v>
+        <f t="shared" ref="G30" si="27">AVERAGE(D30:F30)</f>
+        <v>-1.0064680064680065E-2</v>
       </c>
       <c r="H30" s="107">
-        <v>-0.1</v>
+        <f t="shared" ref="H30" si="28">AVERAGE(E30:G30)</f>
+        <v>-1.6752906752906752E-2</v>
       </c>
       <c r="I30" s="107">
-        <v>-0.1</v>
+        <f t="shared" ref="I30" si="29">AVERAGE(F30:H30)</f>
+        <v>-1.2995559662226328E-2</v>
       </c>
       <c r="J30" s="107">
-        <v>-0.1</v>
+        <f t="shared" ref="J30" si="30">AVERAGE(G30:I30)</f>
+        <v>-1.3271048826604381E-2</v>
       </c>
     </row>
     <row r="32" spans="2:12">
@@ -2389,23 +2404,23 @@
       </c>
       <c r="F32" s="11">
         <f>F25+F27+F28+F29</f>
-        <v>7678609.2800000012</v>
+        <v>539869.86153193773</v>
       </c>
       <c r="G32" s="11">
-        <f t="shared" ref="G32:J32" si="14">G25+G27+G28+G29</f>
-        <v>9397310.2080000024</v>
+        <f t="shared" ref="G32:J32" si="31">G25+G27+G28+G29</f>
+        <v>678922.47228844557</v>
       </c>
       <c r="H32" s="11">
-        <f t="shared" si="14"/>
-        <v>10337041.228800002</v>
+        <f t="shared" si="31"/>
+        <v>1003996.4842043641</v>
       </c>
       <c r="I32" s="11">
-        <f t="shared" si="14"/>
-        <v>11370745.351680005</v>
+        <f t="shared" si="31"/>
+        <v>812100.67074796802</v>
       </c>
       <c r="J32" s="11">
-        <f t="shared" si="14"/>
-        <v>12507819.886848006</v>
+        <f t="shared" si="31"/>
+        <v>915556.68462133419</v>
       </c>
     </row>
     <row r="33" spans="2:10">
@@ -2422,35 +2437,35 @@
       </c>
       <c r="C34" s="9">
         <f>DATA!D8</f>
-        <v>1127000</v>
+        <v>851000</v>
       </c>
       <c r="D34" s="9">
         <f>DATA!C8</f>
-        <v>2422000</v>
+        <v>1563800</v>
       </c>
       <c r="E34" s="9">
         <f>DATA!B8</f>
-        <v>1640000</v>
+        <v>980000</v>
       </c>
       <c r="F34" s="10">
         <f>F15*F35</f>
-        <v>2754840.0000000005</v>
+        <v>1264837.627350898</v>
       </c>
       <c r="G34" s="10">
         <f>G15*G35</f>
-        <v>3030324.0000000009</v>
+        <v>1423362.7670453219</v>
       </c>
       <c r="H34" s="10">
         <f>H15*H35</f>
-        <v>3333356.4000000013</v>
+        <v>1345657.968198081</v>
       </c>
       <c r="I34" s="10">
         <f>I15*I35</f>
-        <v>3666692.0400000014</v>
+        <v>1484284.4795701024</v>
       </c>
       <c r="J34" s="10">
         <f>J15*J35</f>
-        <v>4033361.2440000023</v>
+        <v>1565917.2270312118</v>
       </c>
     </row>
     <row r="35" spans="2:10">
@@ -2459,30 +2474,35 @@
       </c>
       <c r="C35" s="13">
         <f>C34/C15</f>
-        <v>9.4412331406551059E-2</v>
+        <v>0.17692307692307693</v>
       </c>
       <c r="D35" s="13">
         <f>D34/D15</f>
-        <v>0.22885760181423037</v>
+        <v>0.39390428211586903</v>
       </c>
       <c r="E35" s="13">
         <f>E34/E15</f>
-        <v>0.13096949369110367</v>
+        <v>0.20374220374220375</v>
       </c>
       <c r="F35" s="107">
-        <v>0.2</v>
+        <f>AVERAGE(C35:E35)</f>
+        <v>0.25818985426038327</v>
       </c>
       <c r="G35" s="107">
-        <v>0.2</v>
+        <f t="shared" ref="G35" si="32">AVERAGE(D35:F35)</f>
+        <v>0.28527878003948537</v>
       </c>
       <c r="H35" s="107">
-        <v>0.2</v>
+        <f t="shared" ref="H35" si="33">AVERAGE(E35:G35)</f>
+        <v>0.24907027934735745</v>
       </c>
       <c r="I35" s="107">
-        <v>0.2</v>
+        <f t="shared" ref="I35" si="34">AVERAGE(F35:H35)</f>
+        <v>0.26417963788240872</v>
       </c>
       <c r="J35" s="107">
-        <v>0.2</v>
+        <f t="shared" ref="J35" si="35">AVERAGE(G35:I35)</f>
+        <v>0.26617623242308386</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" customHeight="1">
@@ -2495,32 +2515,32 @@
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C37" s="19">
         <f>YEARFRAC($G$8,C8)</f>
-        <v>0.77777777777777779</v>
+        <v>0.73055555555555551</v>
       </c>
       <c r="E37" s="38"/>
       <c r="F37" s="10">
         <f>F32*C37</f>
-        <v>5972251.6622222234</v>
+        <v>394404.92661916558</v>
       </c>
       <c r="G37" s="10">
         <f>G32</f>
-        <v>9397310.2080000024</v>
+        <v>678922.47228844557</v>
       </c>
       <c r="H37" s="10">
         <f>H32</f>
-        <v>10337041.228800002</v>
+        <v>1003996.4842043641</v>
       </c>
       <c r="I37" s="10">
         <f>I32</f>
-        <v>11370745.351680005</v>
+        <v>812100.67074796802</v>
       </c>
       <c r="J37" s="10">
         <f>J32</f>
-        <v>12507819.886848006</v>
+        <v>915556.68462133419</v>
       </c>
     </row>
     <row r="38" spans="2:10">
@@ -2531,23 +2551,23 @@
       <c r="E38" s="6"/>
       <c r="F38" s="11">
         <f>F37/(1+$G$5)^((F13-$G$8)/365)</f>
-        <v>5423579.5232928693</v>
+        <v>369357.86467016354</v>
       </c>
       <c r="G38" s="11">
         <f>G37/(1+$G$5)^((G13-$G$8)/365)</f>
-        <v>7543127.2409059834</v>
+        <v>581261.27676044602</v>
       </c>
       <c r="H38" s="11">
         <f>H37/(1+$G$5)^((H13-$G$8)/365)</f>
-        <v>7331574.0836251639</v>
+        <v>785638.69317837362</v>
       </c>
       <c r="I38" s="11">
         <f>I37/(1+$G$5)^((I13-$G$8)/365)</f>
-        <v>7128364.0370859355</v>
+        <v>580960.66625881672</v>
       </c>
       <c r="J38" s="11">
         <f>J37/(1+$G$5)^((J13-$G$8)/365)</f>
-        <v>6930786.3857927276</v>
+        <v>598781.37901285733</v>
       </c>
     </row>
     <row r="39" spans="2:10">
@@ -2597,14 +2617,14 @@
         <v>29</v>
       </c>
       <c r="C43" s="14">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I43" s="10">
         <f>J17</f>
-        <v>10688407.296600007</v>
+        <v>1065836.1010241969</v>
       </c>
     </row>
     <row r="44" spans="2:10">
@@ -2613,14 +2633,15 @@
       </c>
       <c r="C44" s="10">
         <f>J32*(1+C43)</f>
-        <v>12883054.483453447</v>
+        <v>952178.95200618764</v>
       </c>
       <c r="D44" s="20"/>
       <c r="F44" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I44" s="21">
-        <v>60</v>
+        <f>DATA!F13</f>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="2:10">
@@ -2629,14 +2650,14 @@
       </c>
       <c r="C45" s="10">
         <f>(C44)/(G5-C43)</f>
-        <v>127104499.30612369</v>
+        <v>17685335.191472113</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I45" s="10">
         <f>I43*I44</f>
-        <v>641304437.79600036</v>
+        <v>21316722.020483941</v>
       </c>
     </row>
     <row r="46" spans="2:10">
@@ -2645,14 +2666,14 @@
       </c>
       <c r="C46" s="22">
         <f>C45/(1+$G$5)^(($J$13-$G$8)/365)</f>
-        <v>70430669.879583657</v>
+        <v>11566350.365989702</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I46" s="10">
         <f>I45/(1+$G$5)^(($J$13-$G$8)/365)</f>
-        <v>355357217.07174838</v>
+        <v>13941306.335104978</v>
       </c>
     </row>
     <row r="47" spans="2:10">
@@ -2661,14 +2682,14 @@
       </c>
       <c r="C47" s="10">
         <f>SUM(F38:J38)</f>
-        <v>34357431.270702675</v>
+        <v>2915999.8798806574</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I47" s="10">
         <f>C47</f>
-        <v>34357431.270702675</v>
+        <v>2915999.8798806574</v>
       </c>
     </row>
     <row r="48" spans="2:10">
@@ -2677,14 +2698,14 @@
       </c>
       <c r="C48" s="22">
         <f>SUM(C46:C47)</f>
-        <v>104788101.15028633</v>
+        <v>14482350.245870359</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I48" s="10">
         <f>SUM(I46:I47)</f>
-        <v>389714648.34245104</v>
+        <v>16857306.214985635</v>
       </c>
     </row>
     <row r="50" spans="2:14">
@@ -2701,7 +2722,8 @@
         <v>38</v>
       </c>
       <c r="C51" s="9">
-        <v>5000000</v>
+        <f>DATA!F8</f>
+        <v>3450000</v>
       </c>
       <c r="F51" s="84"/>
       <c r="G51" s="84"/>
@@ -2713,18 +2735,20 @@
         <v>39</v>
       </c>
       <c r="C52" s="9">
-        <v>4000000</v>
+        <f>DATA!F9</f>
+        <v>1170000</v>
       </c>
       <c r="F52" s="83"/>
       <c r="H52" s="83"/>
       <c r="I52" s="85"/>
     </row>
     <row r="53" spans="2:14">
-      <c r="B53" s="109" t="s">
-        <v>95</v>
+      <c r="B53" s="108" t="s">
+        <v>88</v>
       </c>
       <c r="C53" s="9">
-        <v>11000000</v>
+        <f>DATA!F10</f>
+        <v>324400</v>
       </c>
       <c r="F53" s="83"/>
       <c r="H53" s="83"/>
@@ -2735,466 +2759,474 @@
     </row>
     <row r="54" spans="2:14">
       <c r="B54" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C54" s="10">
         <f>SUM(C51:C52) - SUM(C53:C53)</f>
-        <v>-2000000</v>
+        <v>4295600</v>
       </c>
       <c r="F54" s="83"/>
       <c r="G54" s="83"/>
       <c r="I54" s="85"/>
     </row>
     <row r="55" spans="2:14">
+      <c r="C55" s="10"/>
       <c r="F55" s="83"/>
       <c r="G55" s="83"/>
       <c r="I55" s="85"/>
     </row>
     <row r="56" spans="2:14">
-      <c r="B56" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C56" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D56" s="23" t="s">
-        <v>14</v>
-      </c>
       <c r="F56" s="83"/>
       <c r="G56" s="83"/>
-      <c r="H56" s="83"/>
+      <c r="I56" s="85"/>
     </row>
     <row r="57" spans="2:14">
-      <c r="B57" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C57" s="22">
-        <f>C48</f>
-        <v>104788101.15028633</v>
-      </c>
-      <c r="D57" s="10">
-        <f>I48</f>
-        <v>389714648.34245104</v>
-      </c>
+      <c r="B57" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F57" s="83"/>
+      <c r="G57" s="83"/>
+      <c r="H57" s="83"/>
     </row>
     <row r="58" spans="2:14">
       <c r="B58" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C58" s="10">
-        <f>$C$54</f>
-        <v>-2000000</v>
+        <v>43</v>
+      </c>
+      <c r="C58" s="22">
+        <f>C48</f>
+        <v>14482350.245870359</v>
       </c>
       <c r="D58" s="10">
-        <f>$C$54</f>
-        <v>-2000000</v>
+        <f>I48</f>
+        <v>16857306.214985635</v>
       </c>
     </row>
     <row r="59" spans="2:14">
       <c r="B59" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C59" s="22">
-        <f>C57-C58</f>
-        <v>106788101.15028633</v>
-      </c>
-      <c r="D59" s="22">
-        <f>D57-D58</f>
-        <v>391714648.34245104</v>
+        <v>40</v>
+      </c>
+      <c r="C59" s="10">
+        <f>$C$54</f>
+        <v>4295600</v>
+      </c>
+      <c r="D59" s="10">
+        <f>$C$54</f>
+        <v>4295600</v>
       </c>
     </row>
     <row r="60" spans="2:14">
       <c r="B60" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C60" s="9">
-        <v>2490000</v>
-      </c>
-      <c r="D60" s="9">
-        <v>2490000</v>
+        <v>44</v>
+      </c>
+      <c r="C60" s="22">
+        <f>C58-C59</f>
+        <v>10186750.245870359</v>
+      </c>
+      <c r="D60" s="22">
+        <f>D58-D59</f>
+        <v>12561706.214985635</v>
       </c>
     </row>
     <row r="61" spans="2:14">
       <c r="B61" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" s="39">
-        <f>C59/C60</f>
-        <v>42.886787610556759</v>
-      </c>
-      <c r="D61" s="39">
-        <f>D59/D60</f>
-        <v>157.31511981624539</v>
+        <v>45</v>
+      </c>
+      <c r="C61" s="9">
+        <f>DATA!F11</f>
+        <v>52068.085106382976</v>
+      </c>
+      <c r="D61" s="9">
+        <f>C61</f>
+        <v>52068.085106382976</v>
       </c>
     </row>
     <row r="62" spans="2:14">
       <c r="B62" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C62" s="13">
-        <f>C61/$G$6-1</f>
-        <v>0.16350481851754628</v>
-      </c>
-      <c r="D62" s="13">
-        <f>D61/$G$6-1</f>
-        <v>3.2679088392904339</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14">
-      <c r="B64" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="39">
+        <f>C60/C61</f>
+        <v>195.64288229646408</v>
+      </c>
+      <c r="D62" s="39">
+        <f>D60/D61</f>
+        <v>241.25539069316969</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14">
+      <c r="B63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="13">
+        <f>C62/$G$6-1</f>
+        <v>-0.16747709661079113</v>
+      </c>
+      <c r="D63" s="13">
+        <f>D62/$G$6-1</f>
+        <v>2.6618683800722076E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="40"/>
+      <c r="I65" s="40"/>
+      <c r="J65" s="40"/>
+    </row>
+    <row r="67" spans="2:10" ht="17.399999999999999">
+      <c r="B67" s="40"/>
+      <c r="D67" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="46"/>
+      <c r="I67" s="46"/>
+    </row>
+    <row r="68" spans="2:10" ht="15.6">
+      <c r="B68" s="40"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="40"/>
-      <c r="D64" s="40"/>
-      <c r="E64" s="40"/>
-      <c r="F64" s="40"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="40"/>
-      <c r="I64" s="40"/>
-      <c r="J64" s="40"/>
-    </row>
-    <row r="66" spans="2:10" ht="17.399999999999999">
-      <c r="B66" s="40"/>
-      <c r="D66" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="E66" s="46"/>
-      <c r="F66" s="46"/>
-      <c r="G66" s="46"/>
-      <c r="H66" s="46"/>
-      <c r="I66" s="46"/>
-    </row>
-    <row r="67" spans="2:10" ht="15.6">
-      <c r="B67" s="40"/>
-      <c r="D67" s="47"/>
-      <c r="E67" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="F67" s="48"/>
-      <c r="G67" s="48"/>
-      <c r="H67" s="48"/>
-      <c r="I67" s="48"/>
-    </row>
-    <row r="68" spans="2:10">
-      <c r="B68" s="40"/>
-      <c r="D68" s="65">
-        <f>C61</f>
-        <v>42.886787610556759</v>
-      </c>
-      <c r="E68" s="66">
-        <f>F68-0.005</f>
-        <v>1.9999999999999997E-2</v>
-      </c>
-      <c r="F68" s="66">
-        <f>G68-0.005</f>
-        <v>2.4999999999999998E-2</v>
-      </c>
-      <c r="G68" s="67">
-        <f>C43</f>
-        <v>0.03</v>
-      </c>
-      <c r="H68" s="66">
-        <f>G68+0.005</f>
-        <v>3.4999999999999996E-2</v>
-      </c>
-      <c r="I68" s="68">
-        <f>H68+0.005</f>
-        <v>3.9999999999999994E-2</v>
-      </c>
+      <c r="F68" s="48"/>
+      <c r="G68" s="48"/>
+      <c r="H68" s="48"/>
+      <c r="I68" s="48"/>
     </row>
     <row r="69" spans="2:10">
       <c r="B69" s="40"/>
-      <c r="D69" s="63">
-        <f>D70+0.005</f>
-        <v>0.14135797358695676</v>
-      </c>
-      <c r="E69" s="56">
-        <f t="dataTable" ref="E69:I73" dt2D="1" dtr="1" r1="C43" r2="G5" ca="1"/>
-        <v>36.689814663179355</v>
-      </c>
-      <c r="F69" s="56">
-        <v>35.696648087000817</v>
-      </c>
-      <c r="G69" s="56">
-        <v>35.696648087000817</v>
-      </c>
-      <c r="H69" s="56">
-        <v>36.689814663179355</v>
-      </c>
-      <c r="I69" s="72">
-        <v>38.943708335233651</v>
+      <c r="D69" s="65">
+        <f>C62</f>
+        <v>195.64288229646408</v>
+      </c>
+      <c r="E69" s="66">
+        <f>F69-0.005</f>
+        <v>3.0000000000000002E-2</v>
+      </c>
+      <c r="F69" s="66">
+        <f>G69-0.005</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G69" s="67">
+        <f>C43</f>
+        <v>0.04</v>
+      </c>
+      <c r="H69" s="66">
+        <f>G69+0.005</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="I69" s="68">
+        <f>H69+0.005</f>
+        <v>4.9999999999999996E-2</v>
       </c>
     </row>
     <row r="70" spans="2:10">
       <c r="B70" s="40"/>
       <c r="D70" s="63">
         <f>D71+0.005</f>
-        <v>0.13635797358695675</v>
+        <v>0.10384002857154381</v>
       </c>
       <c r="E70" s="56">
-        <v>35.190588779186648</v>
+        <f t="dataTable" ref="E70:I74" dt2D="1" dtr="1" r1="C43" r2="G5" ca="1"/>
+        <v>125.70310367229403</v>
       </c>
       <c r="F70" s="56">
-        <v>34.288080202544826</v>
+        <v>115.26016073244398</v>
       </c>
       <c r="G70" s="56">
-        <v>34.288080202544826</v>
+        <v>115.26016073244398</v>
       </c>
       <c r="H70" s="56">
-        <v>35.190588779186648</v>
+        <v>125.70310367229403</v>
       </c>
       <c r="I70" s="72">
-        <v>37.228295248591969</v>
+        <v>151.49638535374254</v>
       </c>
     </row>
     <row r="71" spans="2:10">
       <c r="B71" s="40"/>
-      <c r="C71" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="D71" s="77">
-        <f>G5</f>
-        <v>0.13135797358695675</v>
+      <c r="D71" s="63">
+        <f>D72+0.005</f>
+        <v>9.8840028571543809E-2</v>
       </c>
       <c r="E71" s="56">
-        <v>35.190588779186648</v>
+        <v>112.2091132681668</v>
       </c>
       <c r="F71" s="56">
-        <v>34.288080202544826</v>
-      </c>
-      <c r="G71" s="57">
-        <v>34.288080202544826</v>
+        <v>103.16566774806813</v>
+      </c>
+      <c r="G71" s="56">
+        <v>103.16566774806813</v>
       </c>
       <c r="H71" s="56">
-        <v>35.190588779186648</v>
+        <v>112.2091132681668</v>
       </c>
       <c r="I71" s="72">
-        <v>37.228295248591969</v>
+        <v>134.23707422411809</v>
       </c>
     </row>
     <row r="72" spans="2:10">
       <c r="B72" s="40"/>
-      <c r="D72" s="63">
-        <f>D71-0.005</f>
-        <v>0.12635797358695675</v>
+      <c r="C72" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" s="77">
+        <f>G5</f>
+        <v>9.3840028571543804E-2</v>
       </c>
       <c r="E72" s="56">
-        <v>36.689814663179355</v>
+        <v>112.2091132681668</v>
       </c>
       <c r="F72" s="56">
-        <v>35.696648087000817</v>
-      </c>
-      <c r="G72" s="56">
-        <v>35.696648087000817</v>
+        <v>103.16566774806813</v>
+      </c>
+      <c r="G72" s="57">
+        <v>103.16566774806813</v>
       </c>
       <c r="H72" s="56">
-        <v>36.689814663179355</v>
+        <v>112.2091132681668</v>
       </c>
       <c r="I72" s="72">
-        <v>38.943708335233651</v>
+        <v>134.23707422411809</v>
       </c>
     </row>
     <row r="73" spans="2:10">
       <c r="B73" s="40"/>
-      <c r="D73" s="64">
+      <c r="D73" s="63">
         <f>D72-0.005</f>
-        <v>0.12135797358695674</v>
-      </c>
-      <c r="E73" s="71">
-        <v>40.096789109583561</v>
-      </c>
-      <c r="F73" s="71">
-        <v>38.881622732704564</v>
-      </c>
-      <c r="G73" s="71">
-        <v>38.881622732704564</v>
-      </c>
-      <c r="H73" s="71">
-        <v>40.096789109583561</v>
-      </c>
-      <c r="I73" s="73">
-        <v>42.886787610556759</v>
+        <v>8.88400285715438E-2</v>
+      </c>
+      <c r="E73" s="56">
+        <v>125.70310367229403</v>
+      </c>
+      <c r="F73" s="56">
+        <v>115.26016073244398</v>
+      </c>
+      <c r="G73" s="56">
+        <v>115.26016073244398</v>
+      </c>
+      <c r="H73" s="56">
+        <v>125.70310367229403</v>
+      </c>
+      <c r="I73" s="72">
+        <v>151.49638535374254</v>
       </c>
     </row>
     <row r="74" spans="2:10">
-      <c r="B74" s="55" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" ht="17.399999999999999">
-      <c r="B75" s="40"/>
-      <c r="D75" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="E75" s="46"/>
-      <c r="F75" s="46"/>
-      <c r="G75" s="46"/>
-      <c r="H75" s="46"/>
-      <c r="I75" s="46"/>
-    </row>
-    <row r="76" spans="2:10" ht="15.6">
+      <c r="B74" s="40"/>
+      <c r="D74" s="64">
+        <f>D73-0.005</f>
+        <v>8.3840028571543795E-2</v>
+      </c>
+      <c r="E74" s="71">
+        <v>159.04532176004358</v>
+      </c>
+      <c r="F74" s="71">
+        <v>144.7337813248019</v>
+      </c>
+      <c r="G74" s="71">
+        <v>144.7337813248019</v>
+      </c>
+      <c r="H74" s="71">
+        <v>159.04532176004358</v>
+      </c>
+      <c r="I74" s="73">
+        <v>195.64288229646408</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10">
+      <c r="B75" s="55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" ht="17.399999999999999">
       <c r="B76" s="40"/>
-      <c r="D76" s="47"/>
-      <c r="E76" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="F76" s="48"/>
-      <c r="G76" s="48"/>
-      <c r="H76" s="48"/>
-      <c r="I76" s="48"/>
-    </row>
-    <row r="77" spans="2:10">
+      <c r="D76" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="E76" s="46"/>
+      <c r="F76" s="46"/>
+      <c r="G76" s="46"/>
+      <c r="H76" s="46"/>
+      <c r="I76" s="46"/>
+    </row>
+    <row r="77" spans="2:10" ht="15.6">
       <c r="B77" s="40"/>
-      <c r="D77" s="51">
-        <f>D61</f>
-        <v>157.31511981624539</v>
-      </c>
-      <c r="E77" s="60">
-        <f>F77-0.5</f>
-        <v>59</v>
-      </c>
-      <c r="F77" s="60">
-        <f>G77-0.5</f>
-        <v>59.5</v>
-      </c>
-      <c r="G77" s="61">
-        <f>I44</f>
-        <v>60</v>
-      </c>
-      <c r="H77" s="60">
-        <f>G77+0.5</f>
-        <v>60.5</v>
-      </c>
-      <c r="I77" s="62">
-        <f>H77+0.5</f>
-        <v>61</v>
-      </c>
-      <c r="J77" s="25"/>
+      <c r="D77" s="47"/>
+      <c r="E77" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="F77" s="48"/>
+      <c r="G77" s="48"/>
+      <c r="H77" s="48"/>
+      <c r="I77" s="48"/>
     </row>
     <row r="78" spans="2:10">
       <c r="B78" s="40"/>
-      <c r="D78" s="58">
-        <f>D79+0.005</f>
-        <v>0.14135797358695676</v>
-      </c>
-      <c r="E78" s="69">
-        <f t="dataTable" ref="E78:I82" dt2D="1" dtr="1" r1="I44" r2="G5" ca="1"/>
-        <v>148.80988919099832</v>
-      </c>
-      <c r="F78" s="69">
-        <v>147.66963267438987</v>
-      </c>
-      <c r="G78" s="69">
-        <v>147.66963267438987</v>
-      </c>
-      <c r="H78" s="69">
-        <v>148.80988919099832</v>
-      </c>
-      <c r="I78" s="74">
-        <v>151.09040222421521</v>
-      </c>
+      <c r="D78" s="51">
+        <f>D62</f>
+        <v>241.25539069316969</v>
+      </c>
+      <c r="E78" s="60">
+        <f>F78-0.5</f>
+        <v>19</v>
+      </c>
+      <c r="F78" s="60">
+        <f>G78-0.5</f>
+        <v>19.5</v>
+      </c>
+      <c r="G78" s="61">
+        <f>I44</f>
+        <v>20</v>
+      </c>
+      <c r="H78" s="60">
+        <f>G78+0.5</f>
+        <v>20.5</v>
+      </c>
+      <c r="I78" s="62">
+        <f>H78+0.5</f>
+        <v>21</v>
+      </c>
+      <c r="J78" s="25"/>
     </row>
     <row r="79" spans="2:10">
       <c r="B79" s="40"/>
       <c r="D79" s="58">
         <f>D80+0.005</f>
-        <v>0.13635797358695675</v>
+        <v>0.10384002857154381</v>
       </c>
       <c r="E79" s="69">
-        <v>145.85979443365233</v>
+        <f t="dataTable" ref="E79:I83" dt2D="1" dtr="1" r1="I44" r2="G5" ca="1"/>
+        <v>215.69126792732294</v>
       </c>
       <c r="F79" s="69">
-        <v>144.74313291451978</v>
+        <v>209.27975409452304</v>
       </c>
       <c r="G79" s="69">
-        <v>144.74313291451978</v>
+        <v>209.27975409452304</v>
       </c>
       <c r="H79" s="69">
-        <v>145.85979443365233</v>
+        <v>215.69126792732294</v>
       </c>
       <c r="I79" s="74">
-        <v>148.09311747191737</v>
+        <v>228.51429559292288</v>
       </c>
     </row>
     <row r="80" spans="2:10">
       <c r="B80" s="40"/>
-      <c r="C80" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="D80" s="59">
-        <f>G5</f>
-        <v>0.13135797358695675</v>
+      <c r="D80" s="58">
+        <f>D81+0.005</f>
+        <v>9.8840028571543809E-2</v>
       </c>
       <c r="E80" s="69">
-        <v>145.85979443365233</v>
+        <v>209.83043950030665</v>
       </c>
       <c r="F80" s="69">
-        <v>144.74313291451978</v>
-      </c>
-      <c r="G80" s="70">
-        <v>144.74313291451978</v>
+        <v>203.55464939301837</v>
+      </c>
+      <c r="G80" s="69">
+        <v>203.55464939301837</v>
       </c>
       <c r="H80" s="69">
-        <v>145.85979443365233</v>
+        <v>209.83043950030665</v>
       </c>
       <c r="I80" s="74">
-        <v>148.09311747191737</v>
+        <v>222.38201971488323</v>
       </c>
     </row>
     <row r="81" spans="2:9">
       <c r="B81" s="40"/>
-      <c r="D81" s="58">
-        <f>D80-0.005</f>
-        <v>0.12635797358695675</v>
+      <c r="C81" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D81" s="59">
+        <f>G5</f>
+        <v>9.3840028571543804E-2</v>
       </c>
       <c r="E81" s="69">
-        <v>148.80988919099832</v>
+        <v>209.83043950030665</v>
       </c>
       <c r="F81" s="69">
-        <v>147.66963267438987</v>
-      </c>
-      <c r="G81" s="69">
-        <v>147.66963267438987</v>
+        <v>203.55464939301837</v>
+      </c>
+      <c r="G81" s="70">
+        <v>203.55464939301837</v>
       </c>
       <c r="H81" s="69">
-        <v>148.80988919099832</v>
+        <v>209.83043950030665</v>
       </c>
       <c r="I81" s="74">
-        <v>151.09040222421521</v>
+        <v>222.38201971488323</v>
       </c>
     </row>
     <row r="82" spans="2:9">
       <c r="B82" s="40"/>
-      <c r="D82" s="54">
+      <c r="D82" s="58">
         <f>D81-0.005</f>
-        <v>0.12135797358695674</v>
-      </c>
-      <c r="E82" s="75">
-        <v>154.93655745298071</v>
-      </c>
-      <c r="F82" s="75">
-        <v>153.74727627134834</v>
-      </c>
-      <c r="G82" s="75">
-        <v>153.74727627134834</v>
-      </c>
-      <c r="H82" s="75">
-        <v>154.93655745298071</v>
-      </c>
-      <c r="I82" s="76">
-        <v>157.31511981624539</v>
+        <v>8.88400285715438E-2</v>
+      </c>
+      <c r="E82" s="69">
+        <v>215.69126792732294</v>
+      </c>
+      <c r="F82" s="69">
+        <v>209.27975409452304</v>
+      </c>
+      <c r="G82" s="69">
+        <v>209.27975409452304</v>
+      </c>
+      <c r="H82" s="69">
+        <v>215.69126792732294</v>
+      </c>
+      <c r="I82" s="74">
+        <v>228.51429559292288</v>
       </c>
     </row>
     <row r="83" spans="2:9">
-      <c r="D83" s="25"/>
-    </row>
-    <row r="85" spans="2:9">
-      <c r="D85" s="49"/>
+      <c r="B83" s="40"/>
+      <c r="D83" s="54">
+        <f>D82-0.005</f>
+        <v>8.3840028571543795E-2</v>
+      </c>
+      <c r="E83" s="75">
+        <v>227.8678171856931</v>
+      </c>
+      <c r="F83" s="75">
+        <v>221.17403043195478</v>
+      </c>
+      <c r="G83" s="75">
+        <v>221.17403043195478</v>
+      </c>
+      <c r="H83" s="75">
+        <v>227.8678171856931</v>
+      </c>
+      <c r="I83" s="76">
+        <v>241.25539069316969</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9">
+      <c r="D84" s="25"/>
+    </row>
+    <row r="86" spans="2:9">
+      <c r="D86" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3202,8 +3234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9391A00-DB94-4A9E-8399-BF29E84BD1F6}">
   <dimension ref="B1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="112" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
@@ -3219,7 +3251,7 @@
   <sheetData>
     <row r="1" spans="2:10">
       <c r="B1" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
@@ -3232,23 +3264,24 @@
     </row>
     <row r="2" spans="2:10">
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4"/>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="4"/>
       <c r="F5" s="36">
-        <v>3.5518000000000001E-2</v>
+        <f>DATA!F7</f>
+        <v>3.0416666666666668E-2</v>
       </c>
       <c r="G5" s="8"/>
       <c r="I5" s="7"/>
@@ -3265,36 +3298,36 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="6"/>
       <c r="F7" s="37">
         <f>F5*(1-F6)</f>
-        <v>2.8059220000000003E-2</v>
+        <v>2.4029166666666667E-2</v>
       </c>
       <c r="G7" s="5"/>
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F9" s="36">
         <f>DATA!F6</f>
-        <v>2.315E-2</v>
+        <v>2.6520000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10" s="41">
         <f>DATA!F5</f>
-        <v>1.22</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F11" s="36">
         <v>0.11</v>
@@ -3302,31 +3335,31 @@
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F12" s="37">
         <f>F9+(F10*(F11-F9))</f>
-        <v>0.129107</v>
+        <v>0.11834800000000001</v>
       </c>
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="2:10">
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" s="44">
-        <f>DCF!G6*DCF!C60</f>
-        <v>91781400</v>
+        <f>DCF!G6*DCF!C61</f>
+        <v>12236000</v>
       </c>
       <c r="F15" s="42">
         <f>E15/(E15+E16)</f>
-        <v>1.0222763289500942</v>
+        <v>0.74015824239638028</v>
       </c>
     </row>
     <row r="16" spans="2:10">
@@ -3335,11 +3368,11 @@
       </c>
       <c r="E16" s="44">
         <f>DCF!C54</f>
-        <v>-2000000</v>
+        <v>4295600</v>
       </c>
       <c r="F16" s="42">
         <f>E16/(E16+E15)</f>
-        <v>-2.2276328950094341E-2</v>
+        <v>0.25984175760361972</v>
       </c>
     </row>
     <row r="17" spans="2:10">
@@ -3351,7 +3384,7 @@
       </c>
       <c r="F18" s="19">
         <f>F7*F16+F12*F15</f>
-        <v>0.13135797358695675</v>
+        <v>9.3840028571543804E-2</v>
       </c>
     </row>
     <row r="20" spans="2:10">

</xml_diff>

<commit_message>
added a new table scraping folder for use in future webscraping applications. It returns the corresponding iteration of each piece of text in a table. No more searching through tables, counting cells, or guess/checking
</commit_message>
<xml_diff>
--- a/PANDAS PROJ/RECDCF.xlsx
+++ b/PANDAS PROJ/RECDCF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Downloads\SPRING SEMESTER 2021-2022\PYTHON\GitHub\steveproject\PANDAS PROJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EAD81E-2A87-4377-BC55-0E7A85402AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF710A59-778D-47E0-8437-849C6B56B7D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{38F17426-425A-4946-BB5F-3622334B00E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{38F17426-425A-4946-BB5F-3622334B00E1}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="WACC" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="CIQWBGuid" hidden="1">"382b6a06-a4b5-45ee-959b-8bdd33d85df3"</definedName>
+    <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.48.1616.5174"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
     <definedName name="IQ_CY">10000</definedName>
@@ -49,7 +51,7 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcMode="manual" iterate="1"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1337,16 +1339,16 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1386,7 +1388,7 @@
       </c>
       <c r="G2" s="78"/>
     </row>
-    <row r="3" spans="1:12" ht="16.2" thickBot="1">
+    <row r="3" spans="1:12" ht="16.5" thickBot="1">
       <c r="A3" s="94" t="s">
         <v>14</v>
       </c>
@@ -1403,10 +1405,10 @@
         <v>74</v>
       </c>
       <c r="F3" s="96">
-        <v>44659</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="16.2" thickBot="1">
+        <v>44691</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16.5" thickBot="1">
       <c r="A4" s="94" t="s">
         <v>16</v>
       </c>
@@ -1423,7 +1425,7 @@
         <v>76</v>
       </c>
       <c r="F4" s="97">
-        <v>235</v>
+        <v>251.19</v>
       </c>
       <c r="H4" s="101" t="s">
         <v>75</v>
@@ -1470,7 +1472,7 @@
         <v>77</v>
       </c>
       <c r="F6" s="97">
-        <v>2.6520000000000002E-2</v>
+        <v>3.0790000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1557,7 +1559,7 @@
         <v>80</v>
       </c>
       <c r="F11" s="110">
-        <v>52068.085106382976</v>
+        <v>51697.917910744858</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1585,7 +1587,7 @@
         <v>82</v>
       </c>
       <c r="F13" s="97">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1602,7 +1604,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16.2" thickBot="1">
+    <row r="15" spans="1:12" ht="16.5" thickBot="1">
       <c r="A15" s="98" t="s">
         <v>86</v>
       </c>
@@ -1679,23 +1681,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF651AB-D597-9D44-826B-59063E0D92DF}">
   <dimension ref="B2:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="1.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="54.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.75" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.25" style="1" customWidth="1"/>
     <col min="7" max="8" width="12.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.75" style="1" customWidth="1"/>
     <col min="11" max="11" width="1.5" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.796875" style="1"/>
+    <col min="12" max="16384" width="10.75" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
@@ -1731,7 +1733,7 @@
       </c>
       <c r="G5" s="36">
         <f>WACC!F18</f>
-        <v>9.3840028571543804E-2</v>
+        <v>9.4582781358979115E-2</v>
       </c>
       <c r="H5" s="19"/>
     </row>
@@ -1748,7 +1750,7 @@
       </c>
       <c r="G6" s="8">
         <f>DATA!F4</f>
-        <v>235</v>
+        <v>251.19</v>
       </c>
       <c r="I6" s="7"/>
     </row>
@@ -1765,7 +1767,7 @@
       </c>
       <c r="G7" s="5">
         <f>DATA!F3</f>
-        <v>44659</v>
+        <v>44691</v>
       </c>
     </row>
     <row r="8" spans="2:12">
@@ -1782,7 +1784,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5">
         <f>G7</f>
-        <v>44659</v>
+        <v>44691</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -2519,12 +2521,12 @@
       </c>
       <c r="C37" s="19">
         <f>YEARFRAC($G$8,C8)</f>
-        <v>0.73055555555555551</v>
+        <v>0.64166666666666672</v>
       </c>
       <c r="E37" s="38"/>
       <c r="F37" s="10">
         <f>F32*C37</f>
-        <v>394404.92661916558</v>
+        <v>346416.49448299338</v>
       </c>
       <c r="G37" s="10">
         <f>G32</f>
@@ -2551,23 +2553,23 @@
       <c r="E38" s="6"/>
       <c r="F38" s="11">
         <f>F37/(1+$G$5)^((F13-$G$8)/365)</f>
-        <v>369357.86467016354</v>
+        <v>326835.26363370282</v>
       </c>
       <c r="G38" s="11">
         <f>G37/(1+$G$5)^((G13-$G$8)/365)</f>
-        <v>581261.27676044602</v>
+        <v>585196.76629274513</v>
       </c>
       <c r="H38" s="11">
         <f>H37/(1+$G$5)^((H13-$G$8)/365)</f>
-        <v>785638.69317837362</v>
+        <v>790419.74956149352</v>
       </c>
       <c r="I38" s="11">
         <f>I37/(1+$G$5)^((I13-$G$8)/365)</f>
-        <v>580960.66625881672</v>
+        <v>584099.51845112478</v>
       </c>
       <c r="J38" s="11">
         <f>J37/(1+$G$5)^((J13-$G$8)/365)</f>
-        <v>598781.37901285733</v>
+        <v>601608.00280654617</v>
       </c>
     </row>
     <row r="39" spans="2:10">
@@ -2617,7 +2619,8 @@
         <v>29</v>
       </c>
       <c r="C43" s="14">
-        <v>0.04</v>
+        <f>DATA!F12</f>
+        <v>0.03</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>30</v>
@@ -2633,7 +2636,7 @@
       </c>
       <c r="C44" s="10">
         <f>J32*(1+C43)</f>
-        <v>952178.95200618764</v>
+        <v>943023.38515997422</v>
       </c>
       <c r="D44" s="20"/>
       <c r="F44" s="1" t="s">
@@ -2641,7 +2644,7 @@
       </c>
       <c r="I44" s="21">
         <f>DATA!F13</f>
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="2:10">
@@ -2650,14 +2653,14 @@
       </c>
       <c r="C45" s="10">
         <f>(C44)/(G5-C43)</f>
-        <v>17685335.191472113</v>
+        <v>14601777.212384848</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I45" s="10">
         <f>I43*I44</f>
-        <v>21316722.020483941</v>
+        <v>15987541.515362954</v>
       </c>
     </row>
     <row r="46" spans="2:10">
@@ -2666,14 +2669,14 @@
       </c>
       <c r="C46" s="22">
         <f>C45/(1+$G$5)^(($J$13-$G$8)/365)</f>
-        <v>11566350.365989702</v>
+        <v>9594759.3128023446</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I46" s="10">
         <f>I45/(1+$G$5)^(($J$13-$G$8)/365)</f>
-        <v>13941306.335104978</v>
+        <v>10505338.535999289</v>
       </c>
     </row>
     <row r="47" spans="2:10">
@@ -2682,14 +2685,14 @@
       </c>
       <c r="C47" s="10">
         <f>SUM(F38:J38)</f>
-        <v>2915999.8798806574</v>
+        <v>2888159.3007456125</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I47" s="10">
         <f>C47</f>
-        <v>2915999.8798806574</v>
+        <v>2888159.3007456125</v>
       </c>
     </row>
     <row r="48" spans="2:10">
@@ -2698,14 +2701,14 @@
       </c>
       <c r="C48" s="22">
         <f>SUM(C46:C47)</f>
-        <v>14482350.245870359</v>
+        <v>12482918.613547957</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I48" s="10">
         <f>SUM(I46:I47)</f>
-        <v>16857306.214985635</v>
+        <v>13393497.836744901</v>
       </c>
     </row>
     <row r="50" spans="2:14">
@@ -2800,11 +2803,11 @@
       </c>
       <c r="C58" s="22">
         <f>C48</f>
-        <v>14482350.245870359</v>
+        <v>12482918.613547957</v>
       </c>
       <c r="D58" s="10">
         <f>I48</f>
-        <v>16857306.214985635</v>
+        <v>13393497.836744901</v>
       </c>
     </row>
     <row r="59" spans="2:14">
@@ -2826,11 +2829,11 @@
       </c>
       <c r="C60" s="22">
         <f>C58-C59</f>
-        <v>10186750.245870359</v>
+        <v>8187318.6135479566</v>
       </c>
       <c r="D60" s="22">
         <f>D58-D59</f>
-        <v>12561706.214985635</v>
+        <v>9097897.8367449008</v>
       </c>
     </row>
     <row r="61" spans="2:14">
@@ -2839,11 +2842,11 @@
       </c>
       <c r="C61" s="9">
         <f>DATA!F11</f>
-        <v>52068.085106382976</v>
+        <v>51697.917910744858</v>
       </c>
       <c r="D61" s="9">
         <f>C61</f>
-        <v>52068.085106382976</v>
+        <v>51697.917910744858</v>
       </c>
     </row>
     <row r="62" spans="2:14">
@@ -2852,11 +2855,11 @@
       </c>
       <c r="C62" s="39">
         <f>C60/C61</f>
-        <v>195.64288229646408</v>
+        <v>158.36844005368175</v>
       </c>
       <c r="D62" s="39">
         <f>D60/D61</f>
-        <v>241.25539069316969</v>
+        <v>175.98190032434556</v>
       </c>
     </row>
     <row r="63" spans="2:14">
@@ -2865,11 +2868,11 @@
       </c>
       <c r="C63" s="13">
         <f>C62/$G$6-1</f>
-        <v>-0.16747709661079113</v>
+        <v>-0.36952728988541839</v>
       </c>
       <c r="D63" s="13">
         <f>D62/$G$6-1</f>
-        <v>2.6618683800722076E-2</v>
+        <v>-0.29940722033382872</v>
       </c>
     </row>
     <row r="65" spans="2:10">
@@ -2885,7 +2888,7 @@
       <c r="I65" s="40"/>
       <c r="J65" s="40"/>
     </row>
-    <row r="67" spans="2:10" ht="17.399999999999999">
+    <row r="67" spans="2:10" ht="19.5">
       <c r="B67" s="40"/>
       <c r="D67" s="53" t="s">
         <v>61</v>
@@ -2896,7 +2899,7 @@
       <c r="H67" s="46"/>
       <c r="I67" s="46"/>
     </row>
-    <row r="68" spans="2:10" ht="15.6">
+    <row r="68" spans="2:10" ht="15.75">
       <c r="B68" s="40"/>
       <c r="D68" s="47"/>
       <c r="E68" s="52" t="s">
@@ -2911,72 +2914,72 @@
       <c r="B69" s="40"/>
       <c r="D69" s="65">
         <f>C62</f>
-        <v>195.64288229646408</v>
+        <v>158.36844005368175</v>
       </c>
       <c r="E69" s="66">
         <f>F69-0.005</f>
-        <v>3.0000000000000002E-2</v>
+        <v>1.9999999999999997E-2</v>
       </c>
       <c r="F69" s="66">
         <f>G69-0.005</f>
-        <v>3.5000000000000003E-2</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="G69" s="67">
         <f>C43</f>
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="H69" s="66">
         <f>G69+0.005</f>
-        <v>4.4999999999999998E-2</v>
+        <v>3.4999999999999996E-2</v>
       </c>
       <c r="I69" s="68">
         <f>H69+0.005</f>
-        <v>4.9999999999999996E-2</v>
+        <v>3.9999999999999994E-2</v>
       </c>
     </row>
     <row r="70" spans="2:10">
       <c r="B70" s="40"/>
       <c r="D70" s="63">
         <f>D71+0.005</f>
-        <v>0.10384002857154381</v>
+        <v>0.10458278135897912</v>
       </c>
       <c r="E70" s="56">
         <f t="dataTable" ref="E70:I74" dt2D="1" dtr="1" r1="C43" r2="G5" ca="1"/>
-        <v>125.70310367229403</v>
+        <v>105.88319275233883</v>
       </c>
       <c r="F70" s="56">
-        <v>115.26016073244398</v>
+        <v>97.752080762228843</v>
       </c>
       <c r="G70" s="56">
-        <v>115.26016073244398</v>
+        <v>97.752080762228843</v>
       </c>
       <c r="H70" s="56">
-        <v>125.70310367229403</v>
+        <v>105.88319275233883</v>
       </c>
       <c r="I70" s="72">
-        <v>151.49638535374254</v>
+        <v>125.41605581652118</v>
       </c>
     </row>
     <row r="71" spans="2:10">
       <c r="B71" s="40"/>
       <c r="D71" s="63">
         <f>D72+0.005</f>
-        <v>9.8840028571543809E-2</v>
+        <v>9.9582781358979119E-2</v>
       </c>
       <c r="E71" s="56">
-        <v>112.2091132681668</v>
+        <v>95.048661813684177</v>
       </c>
       <c r="F71" s="56">
-        <v>103.16566774806813</v>
+        <v>87.896006677174171</v>
       </c>
       <c r="G71" s="56">
-        <v>103.16566774806813</v>
+        <v>87.896006677174171</v>
       </c>
       <c r="H71" s="56">
-        <v>112.2091132681668</v>
+        <v>95.048661813684177</v>
       </c>
       <c r="I71" s="72">
-        <v>134.23707422411809</v>
+        <v>112.050279635034</v>
       </c>
     </row>
     <row r="72" spans="2:10">
@@ -2986,66 +2989,66 @@
       </c>
       <c r="D72" s="77">
         <f>G5</f>
-        <v>9.3840028571543804E-2</v>
+        <v>9.4582781358979115E-2</v>
       </c>
       <c r="E72" s="56">
-        <v>112.2091132681668</v>
+        <v>95.048661813684177</v>
       </c>
       <c r="F72" s="56">
-        <v>103.16566774806813</v>
+        <v>87.896006677174171</v>
       </c>
       <c r="G72" s="57">
-        <v>103.16566774806813</v>
+        <v>87.896006677174171</v>
       </c>
       <c r="H72" s="56">
-        <v>112.2091132681668</v>
+        <v>95.048661813684177</v>
       </c>
       <c r="I72" s="72">
-        <v>134.23707422411809</v>
+        <v>112.050279635034</v>
       </c>
     </row>
     <row r="73" spans="2:10">
       <c r="B73" s="40"/>
       <c r="D73" s="63">
         <f>D72-0.005</f>
-        <v>8.88400285715438E-2</v>
+        <v>8.9582781358979111E-2</v>
       </c>
       <c r="E73" s="56">
-        <v>125.70310367229403</v>
+        <v>105.88319275233883</v>
       </c>
       <c r="F73" s="56">
-        <v>115.26016073244398</v>
+        <v>97.752080762228843</v>
       </c>
       <c r="G73" s="56">
-        <v>115.26016073244398</v>
+        <v>97.752080762228843</v>
       </c>
       <c r="H73" s="56">
-        <v>125.70310367229403</v>
+        <v>105.88319275233883</v>
       </c>
       <c r="I73" s="72">
-        <v>151.49638535374254</v>
+        <v>125.41605581652118</v>
       </c>
     </row>
     <row r="74" spans="2:10">
       <c r="B74" s="40"/>
       <c r="D74" s="64">
         <f>D73-0.005</f>
-        <v>8.3840028571543795E-2</v>
+        <v>8.4582781358979106E-2</v>
       </c>
       <c r="E74" s="71">
-        <v>159.04532176004358</v>
+        <v>131.92403233796034</v>
       </c>
       <c r="F74" s="71">
-        <v>144.7337813248019</v>
+        <v>121.19398890074734</v>
       </c>
       <c r="G74" s="71">
-        <v>144.7337813248019</v>
+        <v>121.19398890074734</v>
       </c>
       <c r="H74" s="71">
-        <v>159.04532176004358</v>
+        <v>131.92403233796034</v>
       </c>
       <c r="I74" s="73">
-        <v>195.64288229646408</v>
+        <v>158.36844005368175</v>
       </c>
     </row>
     <row r="75" spans="2:10">
@@ -3053,7 +3056,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="2:10" ht="17.399999999999999">
+    <row r="76" spans="2:10" ht="19.5">
       <c r="B76" s="40"/>
       <c r="D76" s="53" t="s">
         <v>61</v>
@@ -3064,7 +3067,7 @@
       <c r="H76" s="46"/>
       <c r="I76" s="46"/>
     </row>
-    <row r="77" spans="2:10" ht="15.6">
+    <row r="77" spans="2:10" ht="15.75">
       <c r="B77" s="40"/>
       <c r="D77" s="47"/>
       <c r="E77" s="52" t="s">
@@ -3079,27 +3082,27 @@
       <c r="B78" s="40"/>
       <c r="D78" s="51">
         <f>D62</f>
-        <v>241.25539069316969</v>
+        <v>175.98190032434556</v>
       </c>
       <c r="E78" s="60">
         <f>F78-0.5</f>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F78" s="60">
         <f>G78-0.5</f>
-        <v>19.5</v>
+        <v>14.5</v>
       </c>
       <c r="G78" s="61">
         <f>I44</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H78" s="60">
         <f>G78+0.5</f>
-        <v>20.5</v>
+        <v>15.5</v>
       </c>
       <c r="I78" s="62">
         <f>H78+0.5</f>
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J78" s="25"/>
     </row>
@@ -3107,45 +3110,45 @@
       <c r="B79" s="40"/>
       <c r="D79" s="58">
         <f>D80+0.005</f>
-        <v>0.10384002857154381</v>
+        <v>0.10458278135897912</v>
       </c>
       <c r="E79" s="69">
         <f t="dataTable" ref="E79:I83" dt2D="1" dtr="1" r1="I44" r2="G5" ca="1"/>
-        <v>215.69126792732294</v>
+        <v>153.16866496874934</v>
       </c>
       <c r="F79" s="69">
-        <v>209.27975409452304</v>
+        <v>146.67539639707789</v>
       </c>
       <c r="G79" s="69">
-        <v>209.27975409452304</v>
+        <v>146.67539639707789</v>
       </c>
       <c r="H79" s="69">
-        <v>215.69126792732294</v>
+        <v>153.16866496874934</v>
       </c>
       <c r="I79" s="74">
-        <v>228.51429559292288</v>
+        <v>166.1552021120923</v>
       </c>
     </row>
     <row r="80" spans="2:10">
       <c r="B80" s="40"/>
       <c r="D80" s="58">
         <f>D81+0.005</f>
-        <v>9.8840028571543809E-2</v>
+        <v>9.9582781358979119E-2</v>
       </c>
       <c r="E80" s="69">
-        <v>209.83043950030665</v>
+        <v>148.70470270767325</v>
       </c>
       <c r="F80" s="69">
-        <v>203.55464939301837</v>
+        <v>142.34628010760025</v>
       </c>
       <c r="G80" s="69">
-        <v>203.55464939301837</v>
+        <v>142.34628010760025</v>
       </c>
       <c r="H80" s="69">
-        <v>209.83043950030665</v>
+        <v>148.70470270767325</v>
       </c>
       <c r="I80" s="74">
-        <v>222.38201971488323</v>
+        <v>161.42154790781936</v>
       </c>
     </row>
     <row r="81" spans="2:9">
@@ -3155,66 +3158,66 @@
       </c>
       <c r="D81" s="59">
         <f>G5</f>
-        <v>9.3840028571543804E-2</v>
+        <v>9.4582781358979115E-2</v>
       </c>
       <c r="E81" s="69">
-        <v>209.83043950030665</v>
+        <v>148.70470270767325</v>
       </c>
       <c r="F81" s="69">
-        <v>203.55464939301837</v>
+        <v>142.34628010760025</v>
       </c>
       <c r="G81" s="70">
-        <v>203.55464939301837</v>
+        <v>142.34628010760025</v>
       </c>
       <c r="H81" s="69">
-        <v>209.83043950030665</v>
+        <v>148.70470270767325</v>
       </c>
       <c r="I81" s="74">
-        <v>222.38201971488323</v>
+        <v>161.42154790781936</v>
       </c>
     </row>
     <row r="82" spans="2:9">
       <c r="B82" s="40"/>
       <c r="D82" s="58">
         <f>D81-0.005</f>
-        <v>8.88400285715438E-2</v>
+        <v>8.9582781358979111E-2</v>
       </c>
       <c r="E82" s="69">
-        <v>215.69126792732294</v>
+        <v>153.16866496874934</v>
       </c>
       <c r="F82" s="69">
-        <v>209.27975409452304</v>
+        <v>146.67539639707789</v>
       </c>
       <c r="G82" s="69">
-        <v>209.27975409452304</v>
+        <v>146.67539639707789</v>
       </c>
       <c r="H82" s="69">
-        <v>215.69126792732294</v>
+        <v>153.16866496874934</v>
       </c>
       <c r="I82" s="74">
-        <v>228.51429559292288</v>
+        <v>166.1552021120923</v>
       </c>
     </row>
     <row r="83" spans="2:9">
       <c r="B83" s="40"/>
       <c r="D83" s="54">
         <f>D82-0.005</f>
-        <v>8.3840028571543795E-2</v>
+        <v>8.4582781358979106E-2</v>
       </c>
       <c r="E83" s="75">
-        <v>227.8678171856931</v>
+        <v>162.43481891945996</v>
       </c>
       <c r="F83" s="75">
-        <v>221.17403043195478</v>
+        <v>155.66127821701721</v>
       </c>
       <c r="G83" s="75">
-        <v>221.17403043195478</v>
+        <v>155.66127821701721</v>
       </c>
       <c r="H83" s="75">
-        <v>227.8678171856931</v>
+        <v>162.43481891945996</v>
       </c>
       <c r="I83" s="76">
-        <v>241.25539069316969</v>
+        <v>175.98190032434556</v>
       </c>
     </row>
     <row r="84" spans="2:9">
@@ -3238,15 +3241,15 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="1.5" style="1" customWidth="1"/>
-    <col min="2" max="4" width="8.796875" style="1"/>
-    <col min="5" max="5" width="12.19921875" style="1" customWidth="1"/>
+    <col min="2" max="4" width="8.75" style="1"/>
+    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="8.796875" style="1"/>
+    <col min="7" max="10" width="8.75" style="1"/>
     <col min="11" max="11" width="1.5" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.796875" style="1"/>
+    <col min="12" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
@@ -3313,7 +3316,7 @@
       </c>
       <c r="F9" s="36">
         <f>DATA!F6</f>
-        <v>2.6520000000000002E-2</v>
+        <v>3.0790000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="2:10">
@@ -3339,7 +3342,7 @@
       </c>
       <c r="F12" s="37">
         <f>F9+(F10*(F11-F9))</f>
-        <v>0.11834800000000001</v>
+        <v>0.11792100000000001</v>
       </c>
     </row>
     <row r="14" spans="2:10">
@@ -3355,11 +3358,11 @@
       </c>
       <c r="E15" s="44">
         <f>DCF!G6*DCF!C61</f>
-        <v>12236000</v>
+        <v>12986000</v>
       </c>
       <c r="F15" s="42">
         <f>E15/(E15+E16)</f>
-        <v>0.74015824239638028</v>
+        <v>0.75143505230997132</v>
       </c>
     </row>
     <row r="16" spans="2:10">
@@ -3372,7 +3375,7 @@
       </c>
       <c r="F16" s="42">
         <f>E16/(E16+E15)</f>
-        <v>0.25984175760361972</v>
+        <v>0.24856494769002871</v>
       </c>
     </row>
     <row r="17" spans="2:10">
@@ -3384,7 +3387,7 @@
       </c>
       <c r="F18" s="19">
         <f>F7*F16+F12*F15</f>
-        <v>9.3840028571543804E-2</v>
+        <v>9.4582781358979115E-2</v>
       </c>
     </row>
     <row r="20" spans="2:10">

</xml_diff>

<commit_message>
Added ratios and comps to excel file and scraping
</commit_message>
<xml_diff>
--- a/PANDAS PROJ/RECDCF.xlsx
+++ b/PANDAS PROJ/RECDCF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Downloads\SPRING SEMESTER 2021-2022\PYTHON\GitHub\steveproject\PANDAS PROJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0650BDA-5B44-413B-8E2E-5DCD06209528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FA31DC-322A-4588-B5C2-EA76B5F5B8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{38F17426-425A-4946-BB5F-3622334B00E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{38F17426-425A-4946-BB5F-3622334B00E1}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="DCF" sheetId="1" r:id="rId3"/>
     <sheet name="WACC" sheetId="8" r:id="rId4"/>
     <sheet name="COMPS" sheetId="2" r:id="rId5"/>
-    <sheet name="RATIO ANALYSIS" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="CIQWBGuid" hidden="1">"29e17706-b655-497a-b951-dd160e2824ac"</definedName>
@@ -55,7 +54,6 @@
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -73,8 +71,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="108">
   <si>
     <t>Discounted Cash Flow Valuation</t>
   </si>
@@ -349,28 +369,55 @@
     <t>Comps analysis</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>PE Ratio</t>
-  </si>
-  <si>
-    <t>Market Cap</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beta </t>
-  </si>
-  <si>
     <t>Defaults to a three year average</t>
   </si>
   <si>
-    <t>CSL</t>
-  </si>
-  <si>
-    <t>Carlisle Companies Incorporated (CSL)</t>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>NVIDIA Corporation (NVDA)</t>
+  </si>
+  <si>
+    <t>AVGO</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>QUICK</t>
+  </si>
+  <si>
+    <t>CURRENT</t>
+  </si>
+  <si>
+    <t>DTOE</t>
+  </si>
+  <si>
+    <t>ROA</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>MEDIAN</t>
+  </si>
+  <si>
+    <t>nvda</t>
+  </si>
+  <si>
+    <t>ROE</t>
+  </si>
+  <si>
+    <t>MEAN</t>
   </si>
 </sst>
 </file>
@@ -391,9 +438,16 @@
     <numFmt numFmtId="172" formatCode="_(#,##0.00%_);\(#,##0.00%\);_(&quot;–&quot;_)_%;_(@_)_%"/>
     <numFmt numFmtId="173" formatCode="#,##0.00_);\(#,##0.00\);@_)"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -570,6 +624,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -591,7 +651,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -826,85 +886,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="7" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="7" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -913,70 +988,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="171" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="24" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="24" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -991,77 +1066,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="22" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="23" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="172" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="7" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1440,7 +1501,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1452,108 +1513,108 @@
     <col min="7" max="7" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="16.2" thickBot="1">
       <c r="A1" s="88"/>
       <c r="B1" s="89">
-        <v>44561</v>
+        <v>44592</v>
       </c>
       <c r="C1" s="89">
-        <v>44196</v>
+        <v>44227</v>
       </c>
       <c r="D1" s="89">
-        <v>43830</v>
+        <v>43861</v>
       </c>
       <c r="E1" s="90"/>
       <c r="F1" s="91" t="s">
         <v>67</v>
       </c>
+      <c r="H1" s="99" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="101"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="92" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="93">
-        <v>4810000</v>
+        <v>26910000</v>
       </c>
       <c r="C2" s="93">
-        <v>3970000</v>
+        <v>16680000</v>
       </c>
       <c r="D2" s="93">
-        <v>4810000</v>
+        <v>10920000</v>
       </c>
       <c r="E2" s="84" t="s">
         <v>68</v>
       </c>
       <c r="F2" s="94" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G2" s="77"/>
     </row>
-    <row r="3" spans="1:12" ht="16.2" thickBot="1">
+    <row r="3" spans="1:12">
       <c r="A3" s="92" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="84">
-        <v>837800</v>
+        <v>11850000</v>
       </c>
       <c r="C3" s="84">
-        <v>762200</v>
+        <v>5710000</v>
       </c>
       <c r="D3" s="84">
-        <v>861900</v>
+        <v>3270000</v>
       </c>
       <c r="E3" s="84" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="94">
-        <v>44715</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="16.2" thickBot="1">
+        <v>44722</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="92" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="93">
-        <v>584500</v>
+        <v>10680000</v>
       </c>
       <c r="C4" s="93">
-        <v>509900</v>
+        <v>4610000</v>
       </c>
       <c r="D4" s="93">
-        <v>656500</v>
+        <v>2889000</v>
       </c>
       <c r="E4" s="84" t="s">
         <v>75</v>
       </c>
       <c r="F4" s="95">
-        <v>263.10000000000002</v>
-      </c>
-      <c r="H4" s="99" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="101"/>
+        <v>170.85</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="92" t="s">
         <v>69</v>
       </c>
       <c r="B5" s="93">
-        <v>482500</v>
+        <v>9940000</v>
       </c>
       <c r="C5" s="93">
-        <v>404200</v>
+        <v>4410000</v>
       </c>
       <c r="D5" s="93">
-        <v>595300</v>
+        <v>2970000</v>
       </c>
       <c r="E5" s="84" t="s">
         <v>52</v>
       </c>
       <c r="F5" s="95">
-        <v>0.99</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1561,19 +1622,19 @@
         <v>70</v>
       </c>
       <c r="B6" s="93">
-        <v>95500</v>
+        <v>189000</v>
       </c>
       <c r="C6" s="93">
-        <v>78500</v>
+        <v>77000</v>
       </c>
       <c r="D6" s="93">
-        <v>121600</v>
+        <v>174000</v>
       </c>
       <c r="E6" s="84" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="95">
-        <v>2.9569999999999999E-2</v>
+        <v>3.0440000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1581,19 +1642,19 @@
         <v>71</v>
       </c>
       <c r="B7" s="93">
-        <v>-134800</v>
+        <v>-976000</v>
       </c>
       <c r="C7" s="93">
-        <v>-95500</v>
+        <v>-1130000</v>
       </c>
       <c r="D7" s="93">
-        <v>-88900</v>
+        <v>-489000</v>
       </c>
       <c r="E7" s="84" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="95">
-        <v>3.0416666666666668E-2</v>
+        <v>2.0188195038494439E-2</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1601,19 +1662,19 @@
         <v>72</v>
       </c>
       <c r="B8" s="93">
-        <v>980000</v>
+        <v>24490000</v>
       </c>
       <c r="C8" s="93">
-        <v>1563800</v>
+        <v>12129999.999999998</v>
       </c>
       <c r="D8" s="93">
-        <v>851000</v>
+        <v>11910000</v>
       </c>
       <c r="E8" s="84" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="95">
-        <v>3450000</v>
+        <v>13240000</v>
       </c>
       <c r="G8" s="107"/>
     </row>
@@ -1628,7 +1689,7 @@
         <v>78</v>
       </c>
       <c r="F9" s="95">
-        <v>1170000</v>
+        <v>4340000</v>
       </c>
       <c r="G9" s="107"/>
     </row>
@@ -1643,7 +1704,7 @@
         <v>86</v>
       </c>
       <c r="F10" s="95">
-        <v>324400</v>
+        <v>21210000</v>
       </c>
       <c r="G10" s="107"/>
       <c r="H10" s="84"/>
@@ -1660,7 +1721,7 @@
         <v>79</v>
       </c>
       <c r="F11" s="108">
-        <v>51698.973774230326</v>
+        <v>2493093.3567456836</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1716,7 +1777,7 @@
         <v>85</v>
       </c>
       <c r="F15" s="98" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1783,80 +1844,284 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="14" max="14" width="43.796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="B1">
+    <row r="1" spans="1:14" ht="16.2" thickBot="1">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A2" s="133"/>
+      <c r="B2" s="134" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="134">
+        <v>45.54</v>
+      </c>
+      <c r="D2" s="134">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="E2" s="134">
+        <v>15.03</v>
+      </c>
+      <c r="F2" s="134">
+        <v>4.7</v>
+      </c>
+      <c r="G2" s="134">
+        <v>5.3</v>
+      </c>
+      <c r="H2" s="134">
+        <v>0</v>
+      </c>
+      <c r="I2" s="131">
+        <v>0.224</v>
+      </c>
+      <c r="J2" s="131">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="K2" s="131">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="L2" s="132">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="M2" s="124"/>
+      <c r="N2" s="127" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="135">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="B3" s="136"/>
+      <c r="C3" s="136"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="126"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="135">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>21.23</v>
-      </c>
-      <c r="C2">
-        <v>27.93</v>
-      </c>
-      <c r="D2">
-        <v>14.46</v>
-      </c>
-      <c r="E2">
-        <v>7.22</v>
-      </c>
-      <c r="F2">
-        <v>39.65</v>
-      </c>
-      <c r="G2">
-        <v>19.71</v>
-      </c>
-      <c r="H2">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="I2">
-        <v>21.46</v>
-      </c>
-      <c r="J2">
-        <v>6.95</v>
-      </c>
-      <c r="K2">
-        <v>17.190000000000001</v>
-      </c>
+      <c r="B4" s="136" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="136">
+        <v>26.82</v>
+      </c>
+      <c r="D4" s="136">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="E4" s="136">
+        <v>7.46</v>
+      </c>
+      <c r="F4" s="136">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G4" s="136">
+        <v>2.4</v>
+      </c>
+      <c r="H4" s="136">
+        <v>1.72</v>
+      </c>
+      <c r="I4" s="125">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="J4" s="125">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="K4" s="125">
+        <v>0.128</v>
+      </c>
+      <c r="L4" s="126">
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="135"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="136"/>
+      <c r="L5" s="137"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="135"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="136"/>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="136"/>
+      <c r="J6" s="136"/>
+      <c r="K6" s="136"/>
+      <c r="L6" s="137"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="135"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="136"/>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="136"/>
+      <c r="H7" s="136"/>
+      <c r="I7" s="136"/>
+      <c r="J7" s="136"/>
+      <c r="K7" s="136"/>
+      <c r="L7" s="137"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="135"/>
+      <c r="B8" s="136"/>
+      <c r="C8" s="136"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="136"/>
+      <c r="F8" s="136"/>
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="136"/>
+      <c r="J8" s="136"/>
+      <c r="K8" s="136"/>
+      <c r="L8" s="137"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="135"/>
+      <c r="B9" s="136"/>
+      <c r="C9" s="136"/>
+      <c r="D9" s="136"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
+      <c r="G9" s="136"/>
+      <c r="H9" s="136"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="136"/>
+      <c r="K9" s="136"/>
+      <c r="L9" s="137"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="135"/>
+      <c r="B10" s="136"/>
+      <c r="C10" s="136"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="136"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="136"/>
+      <c r="J10" s="136"/>
+      <c r="K10" s="136"/>
+      <c r="L10" s="137"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="135"/>
+      <c r="B11" s="136"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+      <c r="H11" s="136"/>
+      <c r="I11" s="136"/>
+      <c r="J11" s="136"/>
+      <c r="K11" s="136"/>
+      <c r="L11" s="137"/>
+    </row>
+    <row r="12" spans="1:14" ht="16.2" thickBot="1">
+      <c r="A12" s="138"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="139"/>
+      <c r="L12" s="140"/>
+    </row>
+    <row r="19" spans="7:7">
+      <c r="G19" s="130"/>
+    </row>
+    <row r="20" spans="7:7">
+      <c r="G20" s="130"/>
+    </row>
+    <row r="21" spans="7:7">
+      <c r="G21" s="130"/>
+    </row>
+    <row r="22" spans="7:7">
+      <c r="G22" s="130"/>
+    </row>
+    <row r="23" spans="7:7">
+      <c r="G23" s="130"/>
+    </row>
+    <row r="24" spans="7:7">
+      <c r="G24" s="130"/>
+    </row>
+    <row r="25" spans="7:7">
+      <c r="G25" s="130"/>
+    </row>
+    <row r="26" spans="7:7">
+      <c r="G26" s="130"/>
+    </row>
+    <row r="27" spans="7:7">
+      <c r="G27" s="130"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1867,7 +2132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF651AB-D597-9D44-826B-59063E0D92DF}">
   <dimension ref="B2:N86"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -1919,7 +2184,7 @@
       </c>
       <c r="G5" s="36">
         <f>WACC!F18</f>
-        <v>8.8836645668886133E-2</v>
+        <v>0.15812134931285324</v>
       </c>
       <c r="H5" s="19"/>
     </row>
@@ -1929,14 +2194,14 @@
       </c>
       <c r="C6" s="102" t="str">
         <f>DATA!F2</f>
-        <v>CSL</v>
+        <v>NVDA</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="8">
         <f>DATA!F4</f>
-        <v>263.10000000000002</v>
+        <v>170.85</v>
       </c>
       <c r="I6" s="7"/>
     </row>
@@ -1946,14 +2211,14 @@
       </c>
       <c r="C7" s="5">
         <f>DATA!B1</f>
-        <v>44561</v>
+        <v>44592</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="5">
         <f>DATA!F3</f>
-        <v>44715</v>
+        <v>44722</v>
       </c>
     </row>
     <row r="8" spans="2:12">
@@ -1962,7 +2227,7 @@
       </c>
       <c r="C8" s="6">
         <f>F13</f>
-        <v>44926</v>
+        <v>44957</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>8</v>
@@ -1970,7 +2235,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5">
         <f>G7</f>
-        <v>44715</v>
+        <v>44722</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -1999,35 +2264,35 @@
       </c>
       <c r="C12" s="29">
         <f>D12-1</f>
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="D12" s="29">
         <f>E12-1</f>
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E12" s="29">
         <f>YEAR(E13)</f>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="F12" s="30">
         <f>E12+1</f>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G12" s="30">
         <f t="shared" ref="G12:I12" si="0">F12+1</f>
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="H12" s="30">
         <f t="shared" si="0"/>
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="I12" s="30">
         <f t="shared" si="0"/>
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="J12" s="30">
         <f>I12+1</f>
-        <v>2026</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="13" spans="2:12">
@@ -2036,35 +2301,35 @@
       </c>
       <c r="C13" s="32">
         <f>DATA!D1</f>
-        <v>43830</v>
+        <v>43861</v>
       </c>
       <c r="D13" s="32">
         <f>DATA!C1</f>
-        <v>44196</v>
+        <v>44227</v>
       </c>
       <c r="E13" s="33">
         <f>C7</f>
-        <v>44561</v>
+        <v>44592</v>
       </c>
       <c r="F13" s="33">
         <f>EOMONTH(E13,12)</f>
-        <v>44926</v>
+        <v>44957</v>
       </c>
       <c r="G13" s="33">
         <f>EOMONTH(F13,12)</f>
-        <v>45291</v>
+        <v>45322</v>
       </c>
       <c r="H13" s="33">
         <f t="shared" ref="H13:J13" si="1">EOMONTH(G13,12)</f>
-        <v>45657</v>
+        <v>45688</v>
       </c>
       <c r="I13" s="33">
         <f t="shared" si="1"/>
-        <v>46022</v>
+        <v>46053</v>
       </c>
       <c r="J13" s="33">
         <f t="shared" si="1"/>
-        <v>46387</v>
+        <v>46418</v>
       </c>
       <c r="L13" s="87"/>
     </row>
@@ -2077,35 +2342,35 @@
       </c>
       <c r="C15" s="9">
         <f>DATA!D2</f>
-        <v>4810000</v>
+        <v>10920000</v>
       </c>
       <c r="D15" s="9">
         <f>DATA!C2</f>
-        <v>3970000</v>
+        <v>16680000</v>
       </c>
       <c r="E15" s="9">
         <f>DATA!B2</f>
-        <v>4810000</v>
+        <v>26910000</v>
       </c>
       <c r="F15" s="10">
         <f>E15*(1+F16)</f>
-        <v>4898866.4987405548</v>
+        <v>42259220.195272349</v>
       </c>
       <c r="G15" s="10">
         <f t="shared" ref="G15:J15" si="2">F15*(1+G16)</f>
-        <v>4989374.8383539589</v>
+        <v>66363496.525920272</v>
       </c>
       <c r="H15" s="10">
         <f t="shared" si="2"/>
-        <v>5402723.9690103875</v>
+        <v>105166038.99749525</v>
       </c>
       <c r="I15" s="10">
         <f t="shared" si="2"/>
-        <v>5618466.6292516654</v>
+        <v>165653301.44186279</v>
       </c>
       <c r="J15" s="10">
         <f t="shared" si="2"/>
-        <v>5883009.2107630614</v>
+        <v>261193714.39083168</v>
       </c>
       <c r="K15" s="10"/>
     </row>
@@ -2116,31 +2381,31 @@
       <c r="C16" s="12"/>
       <c r="D16" s="12">
         <f>(D15-C15)/C15</f>
-        <v>-0.17463617463617465</v>
+        <v>0.52747252747252749</v>
       </c>
       <c r="E16" s="12">
         <f>(E15-D15)/D15</f>
-        <v>0.21158690176322417</v>
+        <v>0.61330935251798557</v>
       </c>
       <c r="F16" s="105">
         <f>AVERAGE(C16:E16)</f>
-        <v>1.8475363563524763E-2</v>
+        <v>0.57039093999525647</v>
       </c>
       <c r="G16" s="105">
         <f t="shared" ref="G16" si="3">AVERAGE(D16:F16)</f>
-        <v>1.8475363563524763E-2</v>
+        <v>0.57039093999525647</v>
       </c>
       <c r="H16" s="105">
         <f t="shared" ref="H16" si="4">AVERAGE(E16:G16)</f>
-        <v>8.2845876296757895E-2</v>
+        <v>0.58469707750283284</v>
       </c>
       <c r="I16" s="105">
         <f t="shared" ref="I16" si="5">AVERAGE(F16:H16)</f>
-        <v>3.9932201141269143E-2</v>
+        <v>0.57515965249778189</v>
       </c>
       <c r="J16" s="105">
         <f t="shared" ref="J16" si="6">AVERAGE(G16:I16)</f>
-        <v>4.7084480333850598E-2</v>
+        <v>0.57674922333195699</v>
       </c>
     </row>
     <row r="17" spans="2:12">
@@ -2149,35 +2414,35 @@
       </c>
       <c r="C17" s="9">
         <f>DATA!D3</f>
-        <v>861900</v>
+        <v>3270000</v>
       </c>
       <c r="D17" s="9">
         <f>DATA!C3</f>
-        <v>762200</v>
+        <v>5710000</v>
       </c>
       <c r="E17" s="9">
         <f>DATA!B3</f>
-        <v>837800</v>
+        <v>11850000</v>
       </c>
       <c r="F17" s="10">
         <f>F15*F18</f>
-        <v>890545.1947835664</v>
+        <v>15243371.678705961</v>
       </c>
       <c r="G17" s="10">
         <f t="shared" ref="G17:J17" si="7">G15*G18</f>
-        <v>911317.11075406126</v>
+        <v>25293208.539578013</v>
       </c>
       <c r="H17" s="10">
         <f t="shared" si="7"/>
-        <v>969998.44499027822</v>
+        <v>41442403.506696202</v>
       </c>
       <c r="I17" s="10">
         <f t="shared" si="7"/>
-        <v>1018770.9097975146</v>
+        <v>62722353.017539367</v>
       </c>
       <c r="J17" s="10">
         <f t="shared" si="7"/>
-        <v>1065836.1010241969</v>
+        <v>100458067.33067024</v>
       </c>
     </row>
     <row r="18" spans="2:12">
@@ -2186,35 +2451,35 @@
       </c>
       <c r="C18" s="13">
         <f>C17/C15</f>
-        <v>0.17918918918918919</v>
+        <v>0.29945054945054944</v>
       </c>
       <c r="D18" s="13">
         <f t="shared" ref="D18:E18" si="8">D17/D15</f>
-        <v>0.19198992443324936</v>
+        <v>0.342326139088729</v>
       </c>
       <c r="E18" s="13">
         <f t="shared" si="8"/>
-        <v>0.17417879417879417</v>
+        <v>0.44035674470457081</v>
       </c>
       <c r="F18" s="105">
         <f>AVERAGE(C18:E18)</f>
-        <v>0.18178596926707757</v>
+        <v>0.36071114441461644</v>
       </c>
       <c r="G18" s="105">
         <f t="shared" ref="G18:J18" si="9">AVERAGE(D18:F18)</f>
-        <v>0.18265156262637369</v>
+        <v>0.3811313427359721</v>
       </c>
       <c r="H18" s="105">
         <f t="shared" si="9"/>
-        <v>0.17953877535741514</v>
+        <v>0.39406641061838643</v>
       </c>
       <c r="I18" s="105">
         <f t="shared" si="9"/>
-        <v>0.18132543575028881</v>
+        <v>0.37863629925632497</v>
       </c>
       <c r="J18" s="105">
         <f t="shared" si="9"/>
-        <v>0.18117192457802589</v>
+        <v>0.38461135087022785</v>
       </c>
       <c r="L18" s="7" t="s">
         <v>82</v>
@@ -2226,35 +2491,35 @@
       </c>
       <c r="C19" s="9">
         <f>DATA!D4</f>
-        <v>656500</v>
+        <v>2889000</v>
       </c>
       <c r="D19" s="9">
         <f>DATA!C4</f>
-        <v>509900</v>
+        <v>4610000</v>
       </c>
       <c r="E19" s="9">
         <f>DATA!B4</f>
-        <v>584500</v>
+        <v>10680000</v>
       </c>
       <c r="F19" s="10">
         <f>F15*F20</f>
-        <v>631043.31609166053</v>
+        <v>13210483.256725259</v>
       </c>
       <c r="G19" s="10">
         <f t="shared" ref="G19:J19" si="10">G15*G20</f>
-        <v>629942.01389071054</v>
+        <v>21808445.688538782</v>
       </c>
       <c r="H19" s="10">
         <f t="shared" si="10"/>
-        <v>678201.27854894917</v>
+        <v>36391148.914132521</v>
       </c>
       <c r="I19" s="10">
         <f t="shared" si="10"/>
-        <v>712796.80379550753</v>
+        <v>54514415.597270139</v>
       </c>
       <c r="J19" s="10">
         <f t="shared" si="10"/>
-        <v>742539.68737077643</v>
+        <v>87390514.393376231</v>
       </c>
     </row>
     <row r="20" spans="2:12">
@@ -2263,35 +2528,35 @@
       </c>
       <c r="C20" s="13">
         <f>C19/C15</f>
-        <v>0.13648648648648648</v>
+        <v>0.26456043956043956</v>
       </c>
       <c r="D20" s="13">
         <f>D19/D15</f>
-        <v>0.12843828715365238</v>
+        <v>0.27637889688249401</v>
       </c>
       <c r="E20" s="13">
         <f>E19/E15</f>
-        <v>0.12151767151767152</v>
+        <v>0.39687848383500557</v>
       </c>
       <c r="F20" s="105">
         <f>AVERAGE(C20:E20)</f>
-        <v>0.1288141483859368</v>
+        <v>0.31260594009264636</v>
       </c>
       <c r="G20" s="105">
         <f t="shared" ref="G20" si="11">AVERAGE(D20:F20)</f>
-        <v>0.12625670235242023</v>
+        <v>0.32862110693671531</v>
       </c>
       <c r="H20" s="105">
         <f t="shared" ref="H20" si="12">AVERAGE(E20:G20)</f>
-        <v>0.12552950741867619</v>
+        <v>0.34603517695478908</v>
       </c>
       <c r="I20" s="105">
         <f t="shared" ref="I20" si="13">AVERAGE(F20:H20)</f>
-        <v>0.12686678605234439</v>
+        <v>0.32908740799471697</v>
       </c>
       <c r="J20" s="105">
         <f t="shared" ref="J20" si="14">AVERAGE(G20:I20)</f>
-        <v>0.12621766527448028</v>
+        <v>0.33458123062874051</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -2300,35 +2565,35 @@
       </c>
       <c r="C22" s="9">
         <f>DATA!D5</f>
-        <v>595300</v>
+        <v>2970000</v>
       </c>
       <c r="D22" s="9">
         <f>DATA!C5</f>
-        <v>404200</v>
+        <v>4410000</v>
       </c>
       <c r="E22" s="9">
         <f>DATA!B5</f>
-        <v>482500</v>
+        <v>9940000</v>
       </c>
       <c r="F22" s="85">
         <f>F19</f>
-        <v>631043.31609166053</v>
+        <v>13210483.256725259</v>
       </c>
       <c r="G22" s="85">
         <f t="shared" ref="G22:J22" si="15">G19</f>
-        <v>629942.01389071054</v>
+        <v>21808445.688538782</v>
       </c>
       <c r="H22" s="85">
         <f t="shared" si="15"/>
-        <v>678201.27854894917</v>
+        <v>36391148.914132521</v>
       </c>
       <c r="I22" s="85">
         <f t="shared" si="15"/>
-        <v>712796.80379550753</v>
+        <v>54514415.597270139</v>
       </c>
       <c r="J22" s="85">
         <f t="shared" si="15"/>
-        <v>742539.68737077643</v>
+        <v>87390514.393376231</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -2337,35 +2602,35 @@
       </c>
       <c r="C23" s="9">
         <f>DATA!D6</f>
-        <v>121600</v>
+        <v>174000</v>
       </c>
       <c r="D23" s="9">
         <f>DATA!C6</f>
-        <v>78500</v>
+        <v>77000</v>
       </c>
       <c r="E23" s="9">
         <f>DATA!B6</f>
-        <v>95500</v>
+        <v>189000</v>
       </c>
       <c r="F23" s="85">
         <f>F22*F24</f>
-        <v>125452.46384798236</v>
+        <v>418597.32680607709</v>
       </c>
       <c r="G23" s="85">
         <f t="shared" ref="G23:J23" si="16">G22*G24</f>
-        <v>124085.96024198929</v>
+        <v>495496.28582161077</v>
       </c>
       <c r="H23" s="85">
         <f t="shared" si="16"/>
-        <v>134218.09049768021</v>
+        <v>890627.55547900137</v>
       </c>
       <c r="I23" s="85">
         <f t="shared" si="16"/>
-        <v>141058.84596819282</v>
+        <v>1433381.6869706162</v>
       </c>
       <c r="J23" s="85">
         <f t="shared" si="16"/>
-        <v>146720.37142515319</v>
+        <v>2140710.8397297384</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -2374,35 +2639,35 @@
       </c>
       <c r="C24" s="86">
         <f>C23/C22</f>
-        <v>0.20426675625734925</v>
+        <v>5.8585858585858588E-2</v>
       </c>
       <c r="D24" s="86">
         <f t="shared" ref="D24:E24" si="17">D23/D22</f>
-        <v>0.194210786739238</v>
+        <v>1.7460317460317461E-2</v>
       </c>
       <c r="E24" s="86">
         <f t="shared" si="17"/>
-        <v>0.19792746113989637</v>
+        <v>1.9014084507042252E-2</v>
       </c>
       <c r="F24" s="105">
         <f>AVERAGE(C24:E24)</f>
-        <v>0.19880166804549451</v>
+        <v>3.168675351773944E-2</v>
       </c>
       <c r="G24" s="105">
         <f t="shared" ref="G24" si="18">AVERAGE(D24:F24)</f>
-        <v>0.19697997197487629</v>
+        <v>2.2720385161699719E-2</v>
       </c>
       <c r="H24" s="105">
         <f t="shared" ref="H24" si="19">AVERAGE(E24:G24)</f>
-        <v>0.19790303372008908</v>
+        <v>2.4473741062160468E-2</v>
       </c>
       <c r="I24" s="105">
         <f t="shared" ref="I24" si="20">AVERAGE(F24:H24)</f>
-        <v>0.19789489124681994</v>
+        <v>2.6293626580533209E-2</v>
       </c>
       <c r="J24" s="105">
         <f t="shared" ref="J24" si="21">AVERAGE(G24:I24)</f>
-        <v>0.19759263231392843</v>
+        <v>2.4495917601464464E-2</v>
       </c>
     </row>
     <row r="25" spans="2:12">
@@ -2411,35 +2676,35 @@
       </c>
       <c r="C25" s="79">
         <f>C19*(1-C24)</f>
-        <v>522398.87451705022</v>
+        <v>2719745.4545454546</v>
       </c>
       <c r="D25" s="79">
         <f t="shared" ref="D25:J25" si="22">D19*(1-D24)</f>
-        <v>410871.91984166257</v>
+        <v>4529507.9365079366</v>
       </c>
       <c r="E25" s="79">
         <f t="shared" si="22"/>
-        <v>468811.39896373061</v>
+        <v>10476929.577464789</v>
       </c>
       <c r="F25" s="79">
         <f t="shared" si="22"/>
-        <v>505590.85224367818</v>
+        <v>12791885.929919183</v>
       </c>
       <c r="G25" s="79">
         <f t="shared" si="22"/>
-        <v>505856.05364872125</v>
+        <v>21312949.402717173</v>
       </c>
       <c r="H25" s="79">
         <f t="shared" si="22"/>
-        <v>543983.18805126892</v>
+        <v>35500521.358653516</v>
       </c>
       <c r="I25" s="79">
         <f t="shared" si="22"/>
-        <v>571737.95782731473</v>
+        <v>53081033.910299517</v>
       </c>
       <c r="J25" s="79">
         <f t="shared" si="22"/>
-        <v>595819.31594562321</v>
+        <v>85249803.55364649</v>
       </c>
     </row>
     <row r="27" spans="2:12">
@@ -2448,35 +2713,35 @@
       </c>
       <c r="C27" s="10">
         <f>C17-C19</f>
-        <v>205400</v>
+        <v>381000</v>
       </c>
       <c r="D27" s="10">
         <f>D17-D19</f>
-        <v>252300</v>
+        <v>1100000</v>
       </c>
       <c r="E27" s="10">
         <f t="shared" ref="E27:J27" si="23">E17-E19</f>
-        <v>253300</v>
+        <v>1170000</v>
       </c>
       <c r="F27" s="10">
         <f t="shared" si="23"/>
-        <v>259501.87869190588</v>
+        <v>2032888.4219807014</v>
       </c>
       <c r="G27" s="10">
         <f t="shared" si="23"/>
-        <v>281375.09686335071</v>
+        <v>3484762.8510392308</v>
       </c>
       <c r="H27" s="10">
         <f t="shared" si="23"/>
-        <v>291797.16644132906</v>
+        <v>5051254.5925636813</v>
       </c>
       <c r="I27" s="10">
         <f t="shared" si="23"/>
-        <v>305974.10600200703</v>
+        <v>8207937.4202692285</v>
       </c>
       <c r="J27" s="10">
         <f t="shared" si="23"/>
-        <v>323296.41365342052</v>
+        <v>13067552.937294006</v>
       </c>
     </row>
     <row r="28" spans="2:12">
@@ -2486,31 +2751,31 @@
       <c r="C28" s="10"/>
       <c r="D28" s="10">
         <f t="shared" ref="D28:J28" si="24">C34-D34</f>
-        <v>-712800</v>
+        <v>-219999.99999999814</v>
       </c>
       <c r="E28" s="10">
         <f>D34-E34</f>
-        <v>583800</v>
+        <v>-12360000.000000002</v>
       </c>
       <c r="F28" s="10">
         <f t="shared" si="24"/>
-        <v>-284837.62735089799</v>
+        <v>-13936987.491154082</v>
       </c>
       <c r="G28" s="10">
         <f t="shared" si="24"/>
-        <v>-158525.13969442388</v>
+        <v>-17906880.730468936</v>
       </c>
       <c r="H28" s="10">
         <f t="shared" si="24"/>
-        <v>77704.798847240862</v>
+        <v>-37202733.473966703</v>
       </c>
       <c r="I28" s="10">
         <f t="shared" si="24"/>
-        <v>-138626.5113720214</v>
+        <v>-52658106.20688352</v>
       </c>
       <c r="J28" s="10">
         <f t="shared" si="24"/>
-        <v>-81632.747461109422</v>
+        <v>-81985935.433862031</v>
       </c>
     </row>
     <row r="29" spans="2:12">
@@ -2519,35 +2784,35 @@
       </c>
       <c r="C29" s="9">
         <f>DATA!D7*-1</f>
-        <v>88900</v>
+        <v>489000</v>
       </c>
       <c r="D29" s="9">
         <f>DATA!C7*-1</f>
-        <v>95500</v>
+        <v>1130000</v>
       </c>
       <c r="E29" s="9">
         <f>DATA!B7*-1</f>
-        <v>134800</v>
+        <v>976000</v>
       </c>
       <c r="F29" s="10">
         <f>-(F15*F30)</f>
-        <v>59614.757947251652</v>
+        <v>1000828.841189215</v>
       </c>
       <c r="G29" s="10">
         <f t="shared" ref="G29:J29" si="25">-(G15*G30)</f>
-        <v>50216.461470797411</v>
+        <v>1104999.4063144722</v>
       </c>
       <c r="H29" s="10">
         <f t="shared" si="25"/>
-        <v>90511.330864525298</v>
+        <v>2685339.236430197</v>
       </c>
       <c r="I29" s="10">
         <f t="shared" si="25"/>
-        <v>73015.118290667669</v>
+        <v>3637088.3451435799</v>
       </c>
       <c r="J29" s="10">
         <f t="shared" si="25"/>
-        <v>78073.702483399888</v>
+        <v>5584410.3685861994</v>
       </c>
     </row>
     <row r="30" spans="2:12">
@@ -2556,34 +2821,34 @@
       </c>
       <c r="C30" s="13">
         <f>-(C29/C15)</f>
-        <v>-1.8482328482328482E-2</v>
+        <v>-4.4780219780219781E-2</v>
       </c>
       <c r="D30" s="13">
         <v>0.01</v>
       </c>
       <c r="E30" s="13">
         <f t="shared" ref="E30" si="26">-(E29/E15)</f>
-        <v>-2.8024948024948024E-2</v>
+        <v>-3.6269044964697142E-2</v>
       </c>
       <c r="F30" s="105">
         <f>AVERAGE(C30:E30)</f>
-        <v>-1.2169092169092168E-2</v>
+        <v>-2.3683088248305641E-2</v>
       </c>
       <c r="G30" s="105">
         <f t="shared" ref="G30" si="27">AVERAGE(D30:F30)</f>
-        <v>-1.0064680064680065E-2</v>
+        <v>-1.6650711071000926E-2</v>
       </c>
       <c r="H30" s="105">
         <f t="shared" ref="H30" si="28">AVERAGE(E30:G30)</f>
-        <v>-1.6752906752906752E-2</v>
+        <v>-2.5534281428001238E-2</v>
       </c>
       <c r="I30" s="105">
         <f t="shared" ref="I30" si="29">AVERAGE(F30:H30)</f>
-        <v>-1.2995559662226328E-2</v>
+        <v>-2.1956026915769269E-2</v>
       </c>
       <c r="J30" s="105">
         <f t="shared" ref="J30" si="30">AVERAGE(G30:I30)</f>
-        <v>-1.3271048826604381E-2</v>
+        <v>-2.138033980492381E-2</v>
       </c>
     </row>
     <row r="32" spans="2:12">
@@ -2592,23 +2857,23 @@
       </c>
       <c r="F32" s="11">
         <f>F25+F27+F28+F29</f>
-        <v>539869.86153193773</v>
+        <v>1888615.7019350175</v>
       </c>
       <c r="G32" s="11">
         <f t="shared" ref="G32:J32" si="31">G25+G27+G28+G29</f>
-        <v>678922.47228844557</v>
+        <v>7995830.9296019394</v>
       </c>
       <c r="H32" s="11">
         <f t="shared" si="31"/>
-        <v>1003996.4842043641</v>
+        <v>6034381.7136806911</v>
       </c>
       <c r="I32" s="11">
         <f t="shared" si="31"/>
-        <v>812100.67074796802</v>
+        <v>12267953.468828805</v>
       </c>
       <c r="J32" s="11">
         <f t="shared" si="31"/>
-        <v>915556.68462133419</v>
+        <v>21915831.425664663</v>
       </c>
     </row>
     <row r="33" spans="2:10">
@@ -2625,35 +2890,35 @@
       </c>
       <c r="C34" s="9">
         <f>DATA!D8</f>
-        <v>851000</v>
+        <v>11910000</v>
       </c>
       <c r="D34" s="9">
         <f>DATA!C8</f>
-        <v>1563800</v>
+        <v>12129999.999999998</v>
       </c>
       <c r="E34" s="9">
         <f>DATA!B8</f>
-        <v>980000</v>
+        <v>24490000</v>
       </c>
       <c r="F34" s="10">
         <f>F15*F35</f>
-        <v>1264837.627350898</v>
+        <v>38426987.491154082</v>
       </c>
       <c r="G34" s="10">
         <f>G15*G35</f>
-        <v>1423362.7670453219</v>
+        <v>56333868.221623018</v>
       </c>
       <c r="H34" s="10">
         <f>H15*H35</f>
-        <v>1345657.968198081</v>
+        <v>93536601.695589721</v>
       </c>
       <c r="I34" s="10">
         <f>I15*I35</f>
-        <v>1484284.4795701024</v>
+        <v>146194707.90247324</v>
       </c>
       <c r="J34" s="10">
         <f>J15*J35</f>
-        <v>1565917.2270312118</v>
+        <v>228180643.33633527</v>
       </c>
     </row>
     <row r="35" spans="2:10">
@@ -2662,35 +2927,35 @@
       </c>
       <c r="C35" s="13">
         <f>C34/C15</f>
-        <v>0.17692307692307693</v>
+        <v>1.0906593406593406</v>
       </c>
       <c r="D35" s="13">
         <f>D34/D15</f>
-        <v>0.39390428211586903</v>
+        <v>0.72721822541966419</v>
       </c>
       <c r="E35" s="13">
         <f>E34/E15</f>
-        <v>0.20374220374220375</v>
+        <v>0.91007060572277965</v>
       </c>
       <c r="F35" s="105">
         <f>AVERAGE(C35:E35)</f>
-        <v>0.25818985426038327</v>
+        <v>0.9093160572672615</v>
       </c>
       <c r="G35" s="105">
         <f t="shared" ref="G35" si="32">AVERAGE(D35:F35)</f>
-        <v>0.28527878003948537</v>
+        <v>0.84886829613656845</v>
       </c>
       <c r="H35" s="105">
         <f t="shared" ref="H35" si="33">AVERAGE(E35:G35)</f>
-        <v>0.24907027934735745</v>
+        <v>0.88941831970886998</v>
       </c>
       <c r="I35" s="105">
         <f t="shared" ref="I35" si="34">AVERAGE(F35:H35)</f>
-        <v>0.26417963788240872</v>
+        <v>0.8825342243708999</v>
       </c>
       <c r="J35" s="105">
         <f t="shared" ref="J35" si="35">AVERAGE(G35:I35)</f>
-        <v>0.26617623242308386</v>
+        <v>0.87360694673877948</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="15.75" customHeight="1">
@@ -2707,28 +2972,28 @@
       </c>
       <c r="C37" s="19">
         <f>YEARFRAC($G$8,C8)</f>
-        <v>0.57777777777777772</v>
+        <v>0.64166666666666672</v>
       </c>
       <c r="E37" s="38"/>
       <c r="F37" s="10">
         <f>F32*C37</f>
-        <v>311924.80888511956</v>
+        <v>1211861.7420749697</v>
       </c>
       <c r="G37" s="10">
         <f>G32</f>
-        <v>678922.47228844557</v>
+        <v>7995830.9296019394</v>
       </c>
       <c r="H37" s="10">
         <f>H32</f>
-        <v>1003996.4842043641</v>
+        <v>6034381.7136806911</v>
       </c>
       <c r="I37" s="10">
         <f>I32</f>
-        <v>812100.67074796802</v>
+        <v>12267953.468828805</v>
       </c>
       <c r="J37" s="10">
         <f>J32</f>
-        <v>915556.68462133419</v>
+        <v>21915831.425664663</v>
       </c>
     </row>
     <row r="38" spans="2:10">
@@ -2739,23 +3004,23 @@
       <c r="E38" s="6"/>
       <c r="F38" s="11">
         <f>F37/(1+$G$5)^((F13-$G$8)/365)</f>
-        <v>296949.37961578881</v>
+        <v>1102569.4014631917</v>
       </c>
       <c r="G38" s="11">
         <f>G37/(1+$G$5)^((G13-$G$8)/365)</f>
-        <v>593594.62490733748</v>
+        <v>6281485.9882073179</v>
       </c>
       <c r="H38" s="11">
         <f>H37/(1+$G$5)^((H13-$G$8)/365)</f>
-        <v>806005.43613684457</v>
+        <v>4091691.0598588502</v>
       </c>
       <c r="I38" s="11">
         <f>I37/(1+$G$5)^((I13-$G$8)/365)</f>
-        <v>598760.19224695279</v>
+        <v>7182706.3068783861</v>
       </c>
       <c r="J38" s="11">
         <f>J37/(1+$G$5)^((J13-$G$8)/365)</f>
-        <v>619962.69690016785</v>
+        <v>11079492.617716359</v>
       </c>
     </row>
     <row r="39" spans="2:10">
@@ -2813,7 +3078,7 @@
       </c>
       <c r="I43" s="10">
         <f>J17</f>
-        <v>1065836.1010241969</v>
+        <v>100458067.33067024</v>
       </c>
     </row>
     <row r="44" spans="2:10">
@@ -2822,7 +3087,7 @@
       </c>
       <c r="C44" s="10">
         <f>J32*(1+C43)</f>
-        <v>943023.38515997422</v>
+        <v>22573306.368434604</v>
       </c>
       <c r="D44" s="20"/>
       <c r="F44" s="1" t="s">
@@ -2839,14 +3104,14 @@
       </c>
       <c r="C45" s="10">
         <f>(C44)/(G5-C43)</f>
-        <v>16027823.721750028</v>
+        <v>176186923.4869979</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>25</v>
       </c>
       <c r="I45" s="10">
         <f>I43*I44</f>
-        <v>21316722.020483941</v>
+        <v>2009161346.6134048</v>
       </c>
     </row>
     <row r="46" spans="2:10">
@@ -2855,14 +3120,14 @@
       </c>
       <c r="C46" s="22">
         <f>C45/(1+$G$5)^(($J$13-$G$8)/365)</f>
-        <v>10853126.831886264</v>
+        <v>89070849.296019718</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>33</v>
       </c>
       <c r="I46" s="10">
         <f>I45/(1+$G$5)^(($J$13-$G$8)/365)</f>
-        <v>14434466.696462663</v>
+        <v>1015726388.6204199</v>
       </c>
     </row>
     <row r="47" spans="2:10">
@@ -2871,14 +3136,14 @@
       </c>
       <c r="C47" s="10">
         <f>SUM(F38:J38)</f>
-        <v>2915272.329807092</v>
+        <v>29737945.374124102</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I47" s="10">
         <f>C47</f>
-        <v>2915272.329807092</v>
+        <v>29737945.374124102</v>
       </c>
     </row>
     <row r="48" spans="2:10">
@@ -2887,14 +3152,14 @@
       </c>
       <c r="C48" s="22">
         <f>SUM(C46:C47)</f>
-        <v>13768399.161693355</v>
+        <v>118808794.67014381</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>35</v>
       </c>
       <c r="I48" s="10">
         <f>SUM(I46:I47)</f>
-        <v>17349739.026269756</v>
+        <v>1045464333.9945439</v>
       </c>
     </row>
     <row r="50" spans="2:14">
@@ -2912,7 +3177,7 @@
       </c>
       <c r="C51" s="9">
         <f>DATA!F8</f>
-        <v>3450000</v>
+        <v>13240000</v>
       </c>
       <c r="F51" s="82"/>
       <c r="G51" s="82"/>
@@ -2925,7 +3190,7 @@
       </c>
       <c r="C52" s="9">
         <f>DATA!F9</f>
-        <v>1170000</v>
+        <v>4340000</v>
       </c>
       <c r="F52" s="81"/>
       <c r="H52" s="81"/>
@@ -2937,7 +3202,7 @@
       </c>
       <c r="C53" s="9">
         <f>DATA!F10</f>
-        <v>324400</v>
+        <v>21210000</v>
       </c>
       <c r="F53" s="81"/>
       <c r="H53" s="81"/>
@@ -2952,7 +3217,7 @@
       </c>
       <c r="C54" s="10">
         <f>SUM(C51:C52) - SUM(C53:C53)</f>
-        <v>4295600</v>
+        <v>-3630000</v>
       </c>
       <c r="F54" s="81"/>
       <c r="G54" s="81"/>
@@ -2989,11 +3254,11 @@
       </c>
       <c r="C58" s="22">
         <f>C48</f>
-        <v>13768399.161693355</v>
+        <v>118808794.67014381</v>
       </c>
       <c r="D58" s="10">
         <f>I48</f>
-        <v>17349739.026269756</v>
+        <v>1045464333.9945439</v>
       </c>
     </row>
     <row r="59" spans="2:14">
@@ -3002,11 +3267,11 @@
       </c>
       <c r="C59" s="10">
         <f>$C$54</f>
-        <v>4295600</v>
+        <v>-3630000</v>
       </c>
       <c r="D59" s="10">
         <f>$C$54</f>
-        <v>4295600</v>
+        <v>-3630000</v>
       </c>
     </row>
     <row r="60" spans="2:14">
@@ -3015,11 +3280,11 @@
       </c>
       <c r="C60" s="22">
         <f>C58-C59</f>
-        <v>9472799.1616933551</v>
+        <v>122438794.67014381</v>
       </c>
       <c r="D60" s="22">
         <f>D58-D59</f>
-        <v>13054139.026269756</v>
+        <v>1049094333.9945439</v>
       </c>
     </row>
     <row r="61" spans="2:14">
@@ -3028,11 +3293,11 @@
       </c>
       <c r="C61" s="9">
         <f>DATA!F11</f>
-        <v>51698.973774230326</v>
+        <v>2493093.3567456836</v>
       </c>
       <c r="D61" s="9">
         <f>C61</f>
-        <v>51698.973774230326</v>
+        <v>2493093.3567456836</v>
       </c>
     </row>
     <row r="62" spans="2:14">
@@ -3041,11 +3306,11 @@
       </c>
       <c r="C62" s="39">
         <f>C60/C61</f>
-        <v>183.22992644034127</v>
+        <v>49.111195270267451</v>
       </c>
       <c r="D62" s="39">
         <f>D60/D61</f>
-        <v>252.50286559414596</v>
+        <v>420.80026051008417</v>
       </c>
     </row>
     <row r="63" spans="2:14">
@@ -3054,11 +3319,11 @@
       </c>
       <c r="C63" s="13">
         <f>C62/$G$6-1</f>
-        <v>-0.30357306560113551</v>
+        <v>-0.71254787667388086</v>
       </c>
       <c r="D63" s="13">
         <f>D62/$G$6-1</f>
-        <v>-4.0277971896062525E-2</v>
+        <v>1.4629807463276805</v>
       </c>
     </row>
     <row r="65" spans="2:10">
@@ -3100,7 +3365,7 @@
       <c r="B69" s="40"/>
       <c r="D69" s="64">
         <f>C62</f>
-        <v>183.22992644034127</v>
+        <v>49.111195270267451</v>
       </c>
       <c r="E69" s="65">
         <f>F69-0.005</f>
@@ -3127,45 +3392,45 @@
       <c r="B70" s="40"/>
       <c r="D70" s="62">
         <f>D71+0.005</f>
-        <v>9.8836645668886142E-2</v>
+        <v>0.16812134931285325</v>
       </c>
       <c r="E70" s="55">
         <f t="dataTable" ref="E70:I74" dt2D="1" dtr="1" r1="C43" r2="G5" ca="1"/>
-        <v>120.66558034756801</v>
+        <v>42.450983199760572</v>
       </c>
       <c r="F70" s="55">
-        <v>111.10603972291251</v>
+        <v>41.351379807620731</v>
       </c>
       <c r="G70" s="55">
-        <v>111.10603972291251</v>
+        <v>41.351379807620731</v>
       </c>
       <c r="H70" s="55">
-        <v>120.66558034756801</v>
+        <v>42.450983199760572</v>
       </c>
       <c r="I70" s="71">
-        <v>143.95084685987317</v>
+        <v>44.889024182578765</v>
       </c>
     </row>
     <row r="71" spans="2:10">
       <c r="B71" s="40"/>
       <c r="D71" s="62">
         <f>D72+0.005</f>
-        <v>9.3836645668886137E-2</v>
+        <v>0.16312134931285324</v>
       </c>
       <c r="E71" s="55">
-        <v>108.22161859304782</v>
+        <v>40.768169264597589</v>
       </c>
       <c r="F71" s="55">
-        <v>99.874957156395084</v>
+        <v>39.754026946457245</v>
       </c>
       <c r="G71" s="55">
-        <v>99.874957156395084</v>
+        <v>39.754026946457245</v>
       </c>
       <c r="H71" s="55">
-        <v>108.22161859304782</v>
+        <v>40.768169264597589</v>
       </c>
       <c r="I71" s="71">
-        <v>128.3062093230011</v>
+        <v>43.009030638662566</v>
       </c>
     </row>
     <row r="72" spans="2:10">
@@ -3175,66 +3440,66 @@
       </c>
       <c r="D72" s="76">
         <f>G5</f>
-        <v>8.8836645668886133E-2</v>
+        <v>0.15812134931285324</v>
       </c>
       <c r="E72" s="55">
-        <v>108.22161859304782</v>
+        <v>40.768169264597589</v>
       </c>
       <c r="F72" s="55">
-        <v>99.874957156395084</v>
+        <v>39.754026946457245</v>
       </c>
       <c r="G72" s="56">
-        <v>99.874957156395084</v>
+        <v>39.754026946457245</v>
       </c>
       <c r="H72" s="55">
-        <v>108.22161859304782</v>
+        <v>40.768169264597589</v>
       </c>
       <c r="I72" s="71">
-        <v>128.3062093230011</v>
+        <v>43.009030638662566</v>
       </c>
     </row>
     <row r="73" spans="2:10">
       <c r="B73" s="40"/>
       <c r="D73" s="62">
         <f>D72-0.005</f>
-        <v>8.3836645668886128E-2</v>
+        <v>0.15312134931285323</v>
       </c>
       <c r="E73" s="55">
-        <v>120.66558034756801</v>
+        <v>42.450983199760572</v>
       </c>
       <c r="F73" s="55">
-        <v>111.10603972291251</v>
+        <v>41.351379807620731</v>
       </c>
       <c r="G73" s="55">
-        <v>111.10603972291251</v>
+        <v>41.351379807620731</v>
       </c>
       <c r="H73" s="55">
-        <v>120.66558034756801</v>
+        <v>42.450983199760572</v>
       </c>
       <c r="I73" s="71">
-        <v>143.95084685987317</v>
+        <v>44.889024182578765</v>
       </c>
     </row>
     <row r="74" spans="2:10">
       <c r="B74" s="40"/>
       <c r="D74" s="63">
         <f>D73-0.005</f>
-        <v>7.8836645668886124E-2</v>
+        <v>0.14812134931285323</v>
       </c>
       <c r="E74" s="70">
-        <v>150.99113441197952</v>
+        <v>46.202802325099697</v>
       </c>
       <c r="F74" s="70">
-        <v>138.14641234895561</v>
+        <v>44.901014610492773</v>
       </c>
       <c r="G74" s="70">
-        <v>138.14641234895561</v>
+        <v>44.901014610492773</v>
       </c>
       <c r="H74" s="70">
-        <v>150.99113441197952</v>
+        <v>46.202802325099697</v>
       </c>
       <c r="I74" s="72">
-        <v>183.22992644034127</v>
+        <v>49.111195270267451</v>
       </c>
     </row>
     <row r="75" spans="2:10">
@@ -3268,7 +3533,7 @@
       <c r="B78" s="40"/>
       <c r="D78" s="50">
         <f>D62</f>
-        <v>252.50286559414596</v>
+        <v>420.80026051008417</v>
       </c>
       <c r="E78" s="59">
         <f>F78-0.5</f>
@@ -3296,45 +3561,45 @@
       <c r="B79" s="40"/>
       <c r="D79" s="57">
         <f>D80+0.005</f>
-        <v>9.8836645668886142E-2</v>
+        <v>0.16812134931285325</v>
       </c>
       <c r="E79" s="68">
         <f t="dataTable" ref="E79:I83" dt2D="1" dtr="1" r1="I44" r2="G5" ca="1"/>
-        <v>226.24101431976186</v>
+        <v>384.9343101904883</v>
       </c>
       <c r="F79" s="68">
-        <v>219.54723934720681</v>
+        <v>375.14778802595629</v>
       </c>
       <c r="G79" s="68">
-        <v>219.54723934720681</v>
+        <v>375.14778802595629</v>
       </c>
       <c r="H79" s="68">
-        <v>226.24101431976186</v>
+        <v>384.9343101904883</v>
       </c>
       <c r="I79" s="73">
-        <v>239.6285642648721</v>
+        <v>404.50735451955245</v>
       </c>
     </row>
     <row r="80" spans="2:10">
       <c r="B80" s="40"/>
       <c r="D80" s="57">
         <f>D81+0.005</f>
-        <v>9.3836645668886137E-2</v>
+        <v>0.16312134931285324</v>
       </c>
       <c r="E80" s="68">
-        <v>220.31515563978715</v>
+        <v>377.46265788278896</v>
       </c>
       <c r="F80" s="68">
-        <v>213.75915142949324</v>
+        <v>367.86845068057016</v>
       </c>
       <c r="G80" s="68">
-        <v>213.75915142949324</v>
+        <v>367.86845068057016</v>
       </c>
       <c r="H80" s="68">
-        <v>220.31515563978715</v>
+        <v>377.46265788278896</v>
       </c>
       <c r="I80" s="73">
-        <v>233.42716406037502</v>
+        <v>396.65107228722673</v>
       </c>
     </row>
     <row r="81" spans="2:9">
@@ -3344,66 +3609,66 @@
       </c>
       <c r="D81" s="58">
         <f>G5</f>
-        <v>8.8836645668886133E-2</v>
+        <v>0.15812134931285324</v>
       </c>
       <c r="E81" s="68">
-        <v>220.31515563978715</v>
+        <v>377.46265788278896</v>
       </c>
       <c r="F81" s="68">
-        <v>213.75915142949324</v>
+        <v>367.86845068057016</v>
       </c>
       <c r="G81" s="69">
-        <v>213.75915142949324</v>
+        <v>367.86845068057016</v>
       </c>
       <c r="H81" s="68">
-        <v>220.31515563978715</v>
+        <v>377.46265788278896</v>
       </c>
       <c r="I81" s="73">
-        <v>233.42716406037502</v>
+        <v>396.65107228722673</v>
       </c>
     </row>
     <row r="82" spans="2:9">
       <c r="B82" s="40"/>
       <c r="D82" s="57">
         <f>D81-0.005</f>
-        <v>8.3836645668886128E-2</v>
+        <v>0.15312134931285323</v>
       </c>
       <c r="E82" s="68">
-        <v>226.24101431976186</v>
+        <v>384.9343101904883</v>
       </c>
       <c r="F82" s="68">
-        <v>219.54723934720681</v>
+        <v>375.14778802595629</v>
       </c>
       <c r="G82" s="68">
-        <v>219.54723934720681</v>
+        <v>375.14778802595629</v>
       </c>
       <c r="H82" s="68">
-        <v>226.24101431976186</v>
+        <v>384.9343101904883</v>
       </c>
       <c r="I82" s="73">
-        <v>239.6285642648721</v>
+        <v>404.50735451955245</v>
       </c>
     </row>
     <row r="83" spans="2:9">
       <c r="B83" s="40"/>
       <c r="D83" s="53">
         <f>D82-0.005</f>
-        <v>7.8836645668886124E-2</v>
+        <v>0.14812134931285323</v>
       </c>
       <c r="E83" s="74">
-        <v>238.54275609613339</v>
+        <v>400.42945518359846</v>
       </c>
       <c r="F83" s="74">
-        <v>231.5627013471271</v>
+        <v>390.24405252035569</v>
       </c>
       <c r="G83" s="74">
-        <v>231.5627013471271</v>
+        <v>390.24405252035569</v>
       </c>
       <c r="H83" s="74">
-        <v>238.54275609613339</v>
+        <v>400.42945518359846</v>
       </c>
       <c r="I83" s="75">
-        <v>252.50286559414596</v>
+        <v>420.80026051008417</v>
       </c>
     </row>
     <row r="84" spans="2:9">
@@ -3471,7 +3736,7 @@
       <c r="C5" s="4"/>
       <c r="F5" s="36">
         <f>DATA!F7</f>
-        <v>3.0416666666666668E-2</v>
+        <v>2.0188195038494439E-2</v>
       </c>
       <c r="G5" s="8"/>
       <c r="I5" s="7"/>
@@ -3483,10 +3748,10 @@
       <c r="C6" s="5"/>
       <c r="F6" s="110">
         <f>AVERAGE(DCF!C24:E24)</f>
-        <v>0.19880166804549451</v>
+        <v>3.168675351773944E-2</v>
       </c>
       <c r="G6" s="112" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="2:10">
@@ -3496,7 +3761,7 @@
       <c r="C7" s="6"/>
       <c r="F7" s="37">
         <f>F5*(1-F6)</f>
-        <v>2.4369782596949545E-2</v>
+        <v>1.9548496678341618E-2</v>
       </c>
       <c r="G7" s="113"/>
     </row>
@@ -3509,7 +3774,7 @@
       </c>
       <c r="F9" s="36">
         <f>DATA!F6</f>
-        <v>2.9569999999999999E-2</v>
+        <v>3.0440000000000002E-2</v>
       </c>
       <c r="G9" s="114"/>
     </row>
@@ -3519,7 +3784,7 @@
       </c>
       <c r="F10" s="111">
         <f>DATA!F5</f>
-        <v>0.99</v>
+        <v>1.59</v>
       </c>
       <c r="G10" s="112" t="s">
         <v>89</v>
@@ -3539,7 +3804,7 @@
       </c>
       <c r="F12" s="37">
         <f>F9+(F10*(F11-F9))</f>
-        <v>0.10919570000000001</v>
+        <v>0.15694039999999998</v>
       </c>
     </row>
     <row r="14" spans="2:10">
@@ -3555,11 +3820,11 @@
       </c>
       <c r="E15" s="43">
         <f>DCF!G6*DCF!C61</f>
-        <v>13602000</v>
+        <v>425945000</v>
       </c>
       <c r="F15" s="41">
         <f>E15/(E15+E16)</f>
-        <v>0.75999016627927762</v>
+        <v>1.0085954796774919</v>
       </c>
     </row>
     <row r="16" spans="2:10">
@@ -3568,11 +3833,11 @@
       </c>
       <c r="E16" s="43">
         <f>DCF!C54</f>
-        <v>4295600</v>
+        <v>-3630000</v>
       </c>
       <c r="F16" s="41">
         <f>E16/(E16+E15)</f>
-        <v>0.24000983372072232</v>
+        <v>-8.5954796774919198E-3</v>
       </c>
     </row>
     <row r="17" spans="2:10">
@@ -3584,7 +3849,7 @@
       </c>
       <c r="F18" s="19">
         <f>F7*F16+F12*F15</f>
-        <v>8.8836645668886133E-2</v>
+        <v>0.15812134931285324</v>
       </c>
     </row>
     <row r="20" spans="2:10">
@@ -3605,155 +3870,721 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9391A00-DB94-4A9E-8399-BF29E84BD1F6}">
-  <dimension ref="B1:J20"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="112" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="2.59765625" style="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.59765625" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.8984375" style="138" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.69921875" style="48"/>
+    <col min="2" max="2" width="12.69921875" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" style="123" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.796875" style="48" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.19921875" style="48" customWidth="1"/>
-    <col min="6" max="6" width="12" style="48" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.59765625" style="48" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.69921875" style="48"/>
-    <col min="11" max="11" width="1.5" style="48" customWidth="1"/>
+    <col min="6" max="6" width="12.09765625" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.69921875" style="48" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="8.796875" style="48" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.69921875" style="48" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="8.69921875" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="1" customFormat="1" ht="15" thickBot="1">
-      <c r="B1" s="130" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="15" thickBot="1">
+      <c r="B1" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="133"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-    </row>
-    <row r="2" spans="2:10">
+      <c r="C1" s="121"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+    </row>
+    <row r="2" spans="1:12">
       <c r="B2" s="115"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="129"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" thickBot="1">
-      <c r="B3" s="130" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="130" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="130" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="130" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="130" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="130" t="s">
+      <c r="C2" s="122"/>
+      <c r="D2" s="118"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickBot="1">
+      <c r="B3" s="119" t="str" cm="1">
+        <f t="array" ref="B3:L3">DATA_COMPS!B1:L1</f>
+        <v>Ticker</v>
+      </c>
+      <c r="C3" s="119" t="str">
+        <v>PE</v>
+      </c>
+      <c r="D3" s="119" t="str">
+        <v>PB</v>
+      </c>
+      <c r="E3" s="119" t="str">
+        <v>PS</v>
+      </c>
+      <c r="F3" s="119" t="str">
+        <v>QUICK</v>
+      </c>
+      <c r="G3" s="119" t="str">
+        <v>CURRENT</v>
+      </c>
+      <c r="H3" s="119" t="str">
+        <v>DTOE</v>
+      </c>
+      <c r="I3" s="119" t="str">
+        <v>ROA</v>
+      </c>
+      <c r="J3" s="119" t="str">
+        <v>ROE</v>
+      </c>
+      <c r="K3" s="119" t="str">
+        <v>ROI</v>
+      </c>
+      <c r="L3" s="119" t="str">
+        <v>GM</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="117" customFormat="1" ht="15" thickBot="1">
+      <c r="B4" s="141" t="str" cm="1">
+        <f t="array" ref="B4:L14">DATA_COMPS!B2:L12</f>
+        <v>nvda</v>
+      </c>
+      <c r="C4" s="141">
+        <v>45.54</v>
+      </c>
+      <c r="D4" s="141">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="E4" s="141">
+        <v>15.03</v>
+      </c>
+      <c r="F4" s="141">
+        <v>4.7</v>
+      </c>
+      <c r="G4" s="141">
+        <v>5.3</v>
+      </c>
+      <c r="H4" s="141">
+        <v>0</v>
+      </c>
+      <c r="I4" s="141">
+        <v>0.224</v>
+      </c>
+      <c r="J4" s="141">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="K4" s="141">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="L4" s="142">
+        <v>0.65600000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="117"/>
+      <c r="B5" s="128">
+        <v>0</v>
+      </c>
+      <c r="C5" s="128">
+        <v>0</v>
+      </c>
+      <c r="D5" s="128">
+        <v>0</v>
+      </c>
+      <c r="E5" s="128">
+        <v>0</v>
+      </c>
+      <c r="F5" s="128">
+        <v>0</v>
+      </c>
+      <c r="G5" s="128">
+        <v>0</v>
+      </c>
+      <c r="H5" s="128">
+        <v>0</v>
+      </c>
+      <c r="I5" s="128">
+        <v>0</v>
+      </c>
+      <c r="J5" s="128">
+        <v>0</v>
+      </c>
+      <c r="K5" s="128">
+        <v>0</v>
+      </c>
+      <c r="L5" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="B6" s="128" t="str">
+        <v>AVGO</v>
+      </c>
+      <c r="C6" s="128">
+        <v>26.82</v>
+      </c>
+      <c r="D6" s="128">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="E6" s="128">
+        <v>7.46</v>
+      </c>
+      <c r="F6" s="128">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G6" s="128">
+        <v>2.4</v>
+      </c>
+      <c r="H6" s="128">
+        <v>1.72</v>
+      </c>
+      <c r="I6" s="128">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="J6" s="128">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="K6" s="128">
+        <v>0.128</v>
+      </c>
+      <c r="L6" s="48">
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="117"/>
+      <c r="B7" s="128">
+        <v>0</v>
+      </c>
+      <c r="C7" s="128">
+        <v>0</v>
+      </c>
+      <c r="D7" s="128">
+        <v>0</v>
+      </c>
+      <c r="E7" s="128">
+        <v>0</v>
+      </c>
+      <c r="F7" s="128">
+        <v>0</v>
+      </c>
+      <c r="G7" s="128">
+        <v>0</v>
+      </c>
+      <c r="H7" s="128">
+        <v>0</v>
+      </c>
+      <c r="I7" s="128">
+        <v>0</v>
+      </c>
+      <c r="J7" s="128">
+        <v>0</v>
+      </c>
+      <c r="K7" s="128">
+        <v>0</v>
+      </c>
+      <c r="L7" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" s="128">
+        <v>0</v>
+      </c>
+      <c r="C8" s="128">
+        <v>0</v>
+      </c>
+      <c r="D8" s="128">
+        <v>0</v>
+      </c>
+      <c r="E8" s="128">
+        <v>0</v>
+      </c>
+      <c r="F8" s="128">
+        <v>0</v>
+      </c>
+      <c r="G8" s="128">
+        <v>0</v>
+      </c>
+      <c r="H8" s="128">
+        <v>0</v>
+      </c>
+      <c r="I8" s="128">
+        <v>0</v>
+      </c>
+      <c r="J8" s="128">
+        <v>0</v>
+      </c>
+      <c r="K8" s="128">
+        <v>0</v>
+      </c>
+      <c r="L8" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="117"/>
+      <c r="B9" s="128">
+        <v>0</v>
+      </c>
+      <c r="C9" s="128">
+        <v>0</v>
+      </c>
+      <c r="D9" s="128">
+        <v>0</v>
+      </c>
+      <c r="E9" s="128">
+        <v>0</v>
+      </c>
+      <c r="F9" s="128">
+        <v>0</v>
+      </c>
+      <c r="G9" s="128">
+        <v>0</v>
+      </c>
+      <c r="H9" s="128">
+        <v>0</v>
+      </c>
+      <c r="I9" s="128">
+        <v>0</v>
+      </c>
+      <c r="J9" s="128">
+        <v>0</v>
+      </c>
+      <c r="K9" s="128">
+        <v>0</v>
+      </c>
+      <c r="L9" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="B10" s="128">
+        <v>0</v>
+      </c>
+      <c r="C10" s="128">
+        <v>0</v>
+      </c>
+      <c r="D10" s="128">
+        <v>0</v>
+      </c>
+      <c r="E10" s="128">
+        <v>0</v>
+      </c>
+      <c r="F10" s="128">
+        <v>0</v>
+      </c>
+      <c r="G10" s="128">
+        <v>0</v>
+      </c>
+      <c r="H10" s="128">
+        <v>0</v>
+      </c>
+      <c r="I10" s="128">
+        <v>0</v>
+      </c>
+      <c r="J10" s="128">
+        <v>0</v>
+      </c>
+      <c r="K10" s="128">
+        <v>0</v>
+      </c>
+      <c r="L10" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="117"/>
+      <c r="B11" s="128">
+        <v>0</v>
+      </c>
+      <c r="C11" s="128">
+        <v>0</v>
+      </c>
+      <c r="D11" s="128">
+        <v>0</v>
+      </c>
+      <c r="E11" s="128">
+        <v>0</v>
+      </c>
+      <c r="F11" s="128">
+        <v>0</v>
+      </c>
+      <c r="G11" s="128">
+        <v>0</v>
+      </c>
+      <c r="H11" s="128">
+        <v>0</v>
+      </c>
+      <c r="I11" s="128">
+        <v>0</v>
+      </c>
+      <c r="J11" s="128">
+        <v>0</v>
+      </c>
+      <c r="K11" s="128">
+        <v>0</v>
+      </c>
+      <c r="L11" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" s="128">
+        <v>0</v>
+      </c>
+      <c r="C12" s="128">
+        <v>0</v>
+      </c>
+      <c r="D12" s="128">
+        <v>0</v>
+      </c>
+      <c r="E12" s="128">
+        <v>0</v>
+      </c>
+      <c r="F12" s="128">
+        <v>0</v>
+      </c>
+      <c r="G12" s="128">
+        <v>0</v>
+      </c>
+      <c r="H12" s="128">
+        <v>0</v>
+      </c>
+      <c r="I12" s="128">
+        <v>0</v>
+      </c>
+      <c r="J12" s="128">
+        <v>0</v>
+      </c>
+      <c r="K12" s="128">
+        <v>0</v>
+      </c>
+      <c r="L12" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="B13" s="128">
+        <v>0</v>
+      </c>
+      <c r="C13" s="128">
+        <v>0</v>
+      </c>
+      <c r="D13" s="128">
+        <v>0</v>
+      </c>
+      <c r="E13" s="128">
+        <v>0</v>
+      </c>
+      <c r="F13" s="128">
+        <v>0</v>
+      </c>
+      <c r="G13" s="128">
+        <v>0</v>
+      </c>
+      <c r="H13" s="128">
+        <v>0</v>
+      </c>
+      <c r="I13" s="128">
+        <v>0</v>
+      </c>
+      <c r="J13" s="128">
+        <v>0</v>
+      </c>
+      <c r="K13" s="128">
+        <v>0</v>
+      </c>
+      <c r="L13" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="B14" s="128">
+        <v>0</v>
+      </c>
+      <c r="C14" s="128">
+        <v>0</v>
+      </c>
+      <c r="D14" s="128">
+        <v>0</v>
+      </c>
+      <c r="E14" s="128">
+        <v>0</v>
+      </c>
+      <c r="F14" s="128">
+        <v>0</v>
+      </c>
+      <c r="G14" s="128">
+        <v>0</v>
+      </c>
+      <c r="H14" s="128">
+        <v>0</v>
+      </c>
+      <c r="I14" s="128">
+        <v>0</v>
+      </c>
+      <c r="J14" s="128">
+        <v>0</v>
+      </c>
+      <c r="K14" s="128">
+        <v>0</v>
+      </c>
+      <c r="L14" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" s="128"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="128"/>
+      <c r="G15" s="128"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="128"/>
+      <c r="J15" s="128"/>
+      <c r="K15" s="128"/>
+    </row>
+    <row r="16" spans="1:12" ht="15" thickBot="1">
+      <c r="B16" s="119" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="119" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
-    </row>
-    <row r="4" spans="2:10" s="128" customFormat="1">
-      <c r="B4" s="132" t="str">
-        <f>DATA!F2</f>
-        <v>CSL</v>
-      </c>
-      <c r="C4" s="135" t="str">
-        <f>DATA!F15</f>
-        <v>Carlisle Companies Incorporated (CSL)</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="128"/>
-      <c r="C5" s="136"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="118"/>
-      <c r="I5" s="116"/>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="C6" s="137"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="120"/>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="C7" s="137"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="120"/>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="G8" s="122"/>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="F9" s="117"/>
-      <c r="G9" s="122"/>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="F10" s="123"/>
-      <c r="G10" s="120"/>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="F11" s="117"/>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="F12" s="121"/>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="116"/>
-      <c r="F14" s="116"/>
-      <c r="G14" s="116"/>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="E15" s="124"/>
-      <c r="F15" s="125"/>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="E16" s="124"/>
-      <c r="F16" s="125"/>
-    </row>
-    <row r="17" spans="2:10">
-      <c r="F17" s="116"/>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="116"/>
-      <c r="F18" s="126"/>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="17"/>
-      <c r="E20" s="127"/>
-      <c r="F20" s="127"/>
-      <c r="G20" s="127"/>
-      <c r="H20" s="127"/>
-      <c r="I20" s="127"/>
-      <c r="J20" s="127"/>
+      <c r="D16" s="119" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="119" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="119" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="119" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="119" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="119" t="s">
+        <v>101</v>
+      </c>
+      <c r="J16" s="119" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="L16" s="119" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="129" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="123" cm="1">
+        <f t="array" ref="C17">MEDIAN(IF(C4:C14&lt;&gt;0,C4:C14))</f>
+        <v>36.18</v>
+      </c>
+      <c r="D17" s="123" cm="1">
+        <f t="array" ref="D17">MEDIAN(IF(D4:D14&lt;&gt;0,D4:D14))</f>
+        <v>12.940000000000001</v>
+      </c>
+      <c r="E17" s="123" cm="1">
+        <f t="array" ref="E17">MEDIAN(IF(E4:E14&lt;&gt;0,E4:E14))</f>
+        <v>11.244999999999999</v>
+      </c>
+      <c r="F17" s="123" cm="1">
+        <f t="array" ref="F17">MEDIAN(IF(F4:F14&lt;&gt;0,F4:F14))</f>
+        <v>3.45</v>
+      </c>
+      <c r="G17" s="123" cm="1">
+        <f t="array" ref="G17">MEDIAN(IF(G4:G14&lt;&gt;0,G4:G14))</f>
+        <v>3.8499999999999996</v>
+      </c>
+      <c r="H17" s="123" cm="1">
+        <f t="array" ref="H17">MEDIAN(IF(H4:H14&lt;&gt;0,H4:H14))</f>
+        <v>1.72</v>
+      </c>
+      <c r="I17" s="123" cm="1">
+        <f t="array" ref="I17">MEDIAN(IF(I4:I14&lt;&gt;0,I4:I14))</f>
+        <v>0.155</v>
+      </c>
+      <c r="J17" s="123" cm="1">
+        <f t="array" ref="J17">MEDIAN(IF(J4:J14&lt;&gt;0,J4:J14))</f>
+        <v>0.32750000000000001</v>
+      </c>
+      <c r="K17" s="123" cm="1">
+        <f t="array" ref="K17">MEDIAN(IF(K4:K14&lt;&gt;0,K4:K14))</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="L17" s="123" cm="1">
+        <f t="array" ref="L17">MEDIAN(IF(L4:L14&lt;&gt;0,L4:L14))</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="48" t="str" cm="1">
+        <f t="array" ref="B18:L18">B4:L4</f>
+        <v>nvda</v>
+      </c>
+      <c r="C18" s="123">
+        <v>45.54</v>
+      </c>
+      <c r="D18" s="123">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="E18" s="123">
+        <v>15.03</v>
+      </c>
+      <c r="F18" s="123">
+        <v>4.7</v>
+      </c>
+      <c r="G18" s="123">
+        <v>5.3</v>
+      </c>
+      <c r="H18" s="123">
+        <v>0</v>
+      </c>
+      <c r="I18" s="123">
+        <v>0.224</v>
+      </c>
+      <c r="J18" s="123">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="K18" s="123">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="L18" s="123">
+        <v>0.65600000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="F19" s="116"/>
+    </row>
+    <row r="20" spans="2:12" ht="15" thickBot="1">
+      <c r="B20" s="119" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="119" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="119" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="119" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="119" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="119" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" s="119" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" s="119" t="s">
+        <v>101</v>
+      </c>
+      <c r="J20" s="119" t="s">
+        <v>106</v>
+      </c>
+      <c r="K20" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="L20" s="119" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="129" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="123" cm="1">
+        <f t="array" ref="C21">AVERAGE(IF(C4:C14&lt;&gt;0,C4:C14))</f>
+        <v>36.18</v>
+      </c>
+      <c r="D21" s="123" cm="1">
+        <f t="array" ref="D21">AVERAGE(IF(D4:D14&lt;&gt;0,D4:D14))</f>
+        <v>12.940000000000001</v>
+      </c>
+      <c r="E21" s="123" cm="1">
+        <f t="array" ref="E21">AVERAGE(IF(E4:E14&lt;&gt;0,E4:E14))</f>
+        <v>11.244999999999999</v>
+      </c>
+      <c r="F21" s="123" cm="1">
+        <f t="array" ref="F21">AVERAGE(IF(F4:F14&lt;&gt;0,F4:F14))</f>
+        <v>3.45</v>
+      </c>
+      <c r="G21" s="123" cm="1">
+        <f t="array" ref="G21">AVERAGE(IF(G4:G14&lt;&gt;0,G4:G14))</f>
+        <v>3.8499999999999996</v>
+      </c>
+      <c r="H21" s="123" cm="1">
+        <f t="array" ref="H21">AVERAGE(IF(H4:H14&lt;&gt;0,H4:H14))</f>
+        <v>1.72</v>
+      </c>
+      <c r="I21" s="123" cm="1">
+        <f t="array" ref="I21">AVERAGE(IF(I4:I14&lt;&gt;0,I4:I14))</f>
+        <v>0.155</v>
+      </c>
+      <c r="J21" s="123" cm="1">
+        <f t="array" ref="J21">AVERAGE(IF(J4:J14&lt;&gt;0,J4:J14))</f>
+        <v>0.32750000000000001</v>
+      </c>
+      <c r="K21" s="123" cm="1">
+        <f t="array" ref="K21">AVERAGE(IF(K4:K14&lt;&gt;0,K4:K14))</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="L21" s="123" cm="1">
+        <f t="array" ref="L21">AVERAGE(IF(L4:L14&lt;&gt;0,L4:L14))</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="15.6">
+      <c r="B22" t="str" cm="1">
+        <f t="array" ref="B22:L22">B4:L4</f>
+        <v>nvda</v>
+      </c>
+      <c r="C22">
+        <v>45.54</v>
+      </c>
+      <c r="D22">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="E22">
+        <v>15.03</v>
+      </c>
+      <c r="F22">
+        <v>4.7</v>
+      </c>
+      <c r="G22">
+        <v>5.3</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0.224</v>
+      </c>
+      <c r="J22">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="K22">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="L22">
+        <v>0.65600000000000003</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5537A9A-BCD8-4350-B688-A837E119B93A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>